<commit_message>
update README and participants
</commit_message>
<xml_diff>
--- a/planning/Ageing-workshop-regional-homework-all-regions.xlsx
+++ b/planning/Ageing-workshop-regional-homework-all-regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DA1C15-078F-48BA-9598-B33628B23DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964E8522-3331-438E-A347-9D7FBBF90479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="310">
   <si>
     <t>Region</t>
   </si>
@@ -868,13 +868,109 @@
   </si>
   <si>
     <t>Pacific Ocean Perch</t>
+  </si>
+  <si>
+    <t>5Z</t>
+  </si>
+  <si>
+    <t>1970 - Present</t>
+  </si>
+  <si>
+    <t>4X</t>
+  </si>
+  <si>
+    <t>Silver Hake</t>
+  </si>
+  <si>
+    <t>Brosme brosme</t>
+  </si>
+  <si>
+    <t>4VWX</t>
+  </si>
+  <si>
+    <t>1975 - present</t>
+  </si>
+  <si>
+    <t>Hippoglossus hippoglosus</t>
+  </si>
+  <si>
+    <t>3NOPs4VWX5Zc</t>
+  </si>
+  <si>
+    <t>Annual trawl survey, port sampling, at-sea observers, Industry Survey</t>
+  </si>
+  <si>
+    <t>1995-present</t>
+  </si>
+  <si>
+    <t>Digital Images</t>
+  </si>
+  <si>
+    <t>Arctic Surf Clam</t>
+  </si>
+  <si>
+    <t>Mactromeris polynyma</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>Industry and DFO staff collections</t>
+  </si>
+  <si>
+    <t>Sectioned Shell</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Sea Scallop</t>
+  </si>
+  <si>
+    <t>Placopecten magellanicus</t>
+  </si>
+  <si>
+    <t>Industry Survey and staff collections</t>
+  </si>
+  <si>
+    <t>Whole Shell</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Staff collections</t>
+  </si>
+  <si>
+    <t>Mounted Scale</t>
+  </si>
+  <si>
+    <t>1950? - present</t>
+  </si>
+  <si>
+    <t>1970? - present</t>
+  </si>
+  <si>
+    <t>otolith / Scales</t>
+  </si>
+  <si>
+    <t>1980? - Present</t>
+  </si>
+  <si>
+    <t>American Eel</t>
+  </si>
+  <si>
+    <t>Anguilla rostrata</t>
+  </si>
+  <si>
+    <t>1980 - Present</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -954,6 +1050,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="19.8"/>
+      <color rgb="FF333333"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1031,7 +1133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1106,6 +1208,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1165,8 +1272,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}" name="Table2" displayName="Table2" ref="B4:K57" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B4:K57" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}" name="Table2" displayName="Table2" ref="B4:K69" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="B4:K69" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{1D9501B6-DF5E-4720-AD38-3FC53A5D3D5A}" name="Region" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{66C9233C-1717-4818-BD53-313537655389}" name="Species common name" dataDxfId="8"/>
@@ -1446,11 +1553,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1955,96 +2060,110 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="C19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>146</v>
+        <v>38</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>150</v>
+        <v>27</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>152</v>
+        <v>279</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>37</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>12</v>
+        <v>251</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>278</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>156</v>
+        <v>279</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>158</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="K21" s="12"/>
     </row>
     <row r="22" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>160</v>
+        <v>251</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>15</v>
@@ -2052,487 +2171,457 @@
       <c r="G22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>24</v>
+      <c r="H22" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>161</v>
+        <v>279</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>36</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>158</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="J24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>162</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="F26" s="9" t="s">
-        <v>15</v>
+        <v>292</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>101</v>
+        <v>298</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>299</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>164</v>
+        <v>295</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="K26" s="12"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>162</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>101</v>
+        <v>301</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>302</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>165</v>
+        <v>303</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K27" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>162</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>101</v>
+        <v>301</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>302</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>166</v>
+        <v>304</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>162</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" s="9"/>
       <c r="F29" s="9" t="s">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>101</v>
+        <v>301</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>302</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>167</v>
+        <v>304</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>162</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="9"/>
       <c r="F30" s="9" t="s">
-        <v>15</v>
+        <v>305</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>163</v>
+        <v>301</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="I30" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="J30" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" s="12"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>156</v>
-      </c>
       <c r="J34" s="9" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>82</v>
+        <v>65</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>70</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>15</v>
@@ -2544,10 +2633,10 @@
         <v>101</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>108</v>
@@ -2558,10 +2647,10 @@
         <v>19</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>83</v>
+        <v>262</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>162</v>
@@ -2576,10 +2665,10 @@
         <v>101</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K39" s="12" t="s">
         <v>108</v>
@@ -2590,10 +2679,10 @@
         <v>19</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>84</v>
+        <v>263</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>162</v>
@@ -2608,7 +2697,7 @@
         <v>101</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>110</v>
@@ -2622,13 +2711,13 @@
         <v>19</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>15</v>
@@ -2640,10 +2729,10 @@
         <v>101</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="K41" s="12" t="s">
         <v>108</v>
@@ -2653,14 +2742,14 @@
       <c r="B42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>172</v>
+      <c r="C42" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>15</v>
@@ -2672,22 +2761,24 @@
         <v>101</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K42" s="12"/>
+      <c r="K42" s="12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>116</v>
+      <c r="C43" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>168</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>162</v>
@@ -2702,27 +2793,25 @@
         <v>101</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K43" s="12" t="s">
-        <v>108</v>
-      </c>
+      <c r="K43" s="12"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>64</v>
+        <v>275</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>15</v>
@@ -2734,42 +2823,42 @@
         <v>101</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="K44" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>63</v>
+        <v>274</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="K45" s="12" t="s">
         <v>108</v>
@@ -2780,13 +2869,13 @@
         <v>19</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>62</v>
+        <v>273</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>15</v>
@@ -2798,10 +2887,10 @@
         <v>101</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K46" s="12" t="s">
         <v>108</v>
@@ -2811,61 +2900,61 @@
       <c r="B47" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>123</v>
+      <c r="C47" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>78</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="K47" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>89</v>
+      <c r="C48" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K48" s="12" t="s">
         <v>108</v>
@@ -2875,29 +2964,29 @@
       <c r="B49" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>90</v>
+      <c r="C49" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K49" s="12" t="s">
         <v>108</v>
@@ -2907,29 +2996,29 @@
       <c r="B50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>91</v>
+      <c r="C50" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K50" s="12" t="s">
         <v>108</v>
@@ -2939,29 +3028,29 @@
       <c r="B51" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>92</v>
+      <c r="C51" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="K51" s="12" t="s">
         <v>108</v>
@@ -2971,125 +3060,123 @@
       <c r="B52" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>93</v>
+      <c r="C52" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K52" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>94</v>
+      <c r="C53" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K53" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>95</v>
+      <c r="C54" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="K54" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="K54" s="12"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>96</v>
+      <c r="C55" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>116</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>198</v>
+        <v>101</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="K55" s="12" t="s">
         <v>108</v>
@@ -3099,438 +3186,448 @@
       <c r="B56" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>97</v>
+      <c r="C56" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K56" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G57" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="H57" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="I57" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="J57" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="K57" s="22" t="s">
+      <c r="C57" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K57" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B58" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>203</v>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>88</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>206</v>
+        <v>101</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B59" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>147</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>123</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>206</v>
+        <v>105</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B60" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>27</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>210</v>
+        <v>103</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="J60" s="9"/>
+        <v>183</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>115</v>
+      </c>
       <c r="K60" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B61" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>29</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B61" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>20</v>
+        <v>177</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J61" s="9"/>
+        <v>185</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="K61" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="D62" s="23" t="s">
-        <v>214</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>20</v>
+        <v>177</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>216</v>
+        <v>104</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J62" s="24" t="s">
-        <v>36</v>
+        <v>187</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B63" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>28</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>219</v>
+        <v>104</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="J63" s="9"/>
+        <v>189</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="K63" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B64" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E64" s="25" t="s">
-        <v>221</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B64" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G64" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="I64" s="25" t="s">
-        <v>224</v>
+      <c r="G64" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K64" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B65" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>226</v>
+        <v>107</v>
+      </c>
+      <c r="K64" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>228</v>
+        <v>99</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>229</v>
+        <v>20</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>230</v>
+        <v>104</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="J65" s="24" t="s">
-        <v>36</v>
+        <v>193</v>
+      </c>
+      <c r="J65" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="K65" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B66" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>232</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>234</v>
+        <v>126</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>235</v>
+        <v>109</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B67" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="E67" s="9"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B67" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>196</v>
+      </c>
       <c r="F67" s="9" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>47</v>
+        <v>197</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="I67" s="9"/>
+        <v>198</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>199</v>
+      </c>
       <c r="J67" s="9" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B68" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>241</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B68" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>242</v>
+        <v>194</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>47</v>
+        <v>197</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>239</v>
+        <v>200</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B69" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="H69" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="I69" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J69" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K69" s="12" t="s">
-        <v>35</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B69" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I69" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="J69" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="K69" s="22" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -3538,22 +3635,22 @@
         <v>16</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>32</v>
+        <v>203</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>47</v>
+        <v>205</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
       <c r="I70" s="9" t="s">
         <v>167</v>
@@ -3570,25 +3667,25 @@
         <v>16</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>246</v>
+        <v>146</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>248</v>
+        <v>207</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>47</v>
+        <v>208</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>249</v>
+        <v>206</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="J71" s="9" t="s">
         <v>37</v>
@@ -3602,31 +3699,29 @@
         <v>16</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>251</v>
+        <v>38</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>252</v>
+        <v>20</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>249</v>
+        <v>210</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J72" s="9" t="s">
-        <v>37</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="J72" s="9"/>
       <c r="K72" s="12" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -3634,30 +3729,406 @@
         <v>16</v>
       </c>
       <c r="C73" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J73" s="9"/>
+      <c r="K73" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B74" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="I74" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J74" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K74" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B75" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="J75" s="9"/>
+      <c r="K75" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B76" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G76" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="I76" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="J76" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K76" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B77" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="I77" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J77" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K77" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B78" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="J78" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K78" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B79" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K79" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B80" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="I80" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J80" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K80" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B81" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="I81" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J81" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K81" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B82" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H82" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="I82" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J82" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K82" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B83" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H83" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="I83" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J83" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K83" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B84" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="I84" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J84" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K84" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B85" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="D73" s="10" t="s">
+      <c r="D85" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E85" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="F73" s="9" t="s">
+      <c r="F85" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="G85" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="H73" s="9" t="s">
+      <c r="H85" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="I73" s="9" t="s">
+      <c r="I85" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="J73" s="9" t="s">
+      <c r="J85" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K73" s="12" t="s">
+      <c r="K85" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3665,8 +4136,8 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J7" r:id="rId1" xr:uid="{AE9870F2-46B7-4F0E-BEAD-2C74FAC27E5A}"/>
-    <hyperlink ref="J62" r:id="rId2" xr:uid="{192468E9-F3F8-48E1-A457-9E87E99A73CC}"/>
-    <hyperlink ref="J65" r:id="rId3" xr:uid="{9361AF13-362F-4D8A-9FCB-B8CB2E1CB121}"/>
+    <hyperlink ref="J74" r:id="rId2" xr:uid="{192468E9-F3F8-48E1-A457-9E87E99A73CC}"/>
+    <hyperlink ref="J77" r:id="rId3" xr:uid="{9361AF13-362F-4D8A-9FCB-B8CB2E1CB121}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
add to beamer talks
</commit_message>
<xml_diff>
--- a/planning/Ageing-workshop-regional-homework-all-regions.xlsx
+++ b/planning/Ageing-workshop-regional-homework-all-regions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964E8522-3331-438E-A347-9D7FBBF90479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54689889-E98A-414B-910A-0FDD216A215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="307">
   <si>
     <t>Region</t>
   </si>
@@ -432,9 +432,6 @@
     <t>scale on slide</t>
   </si>
   <si>
-    <t>1983 To 2022</t>
-  </si>
-  <si>
     <t>Atlantic Salmon</t>
   </si>
   <si>
@@ -447,9 +444,6 @@
     <t>Annual monitoring surveys (Rotary Screw Traps, Backpack electrofishing, Trap nets)</t>
   </si>
   <si>
-    <t>1973 To 2022</t>
-  </si>
-  <si>
     <t>Blueback Herring</t>
   </si>
   <si>
@@ -873,9 +867,6 @@
     <t>5Z</t>
   </si>
   <si>
-    <t>1970 - Present</t>
-  </si>
-  <si>
     <t>4X</t>
   </si>
   <si>
@@ -912,9 +903,6 @@
     <t>Mactromeris polynyma</t>
   </si>
   <si>
-    <t>Shell</t>
-  </si>
-  <si>
     <t>Industry and DFO staff collections</t>
   </si>
   <si>
@@ -936,9 +924,6 @@
     <t>Whole Shell</t>
   </si>
   <si>
-    <t>Scale</t>
-  </si>
-  <si>
     <t>Staff collections</t>
   </si>
   <si>
@@ -964,6 +949,12 @@
   </si>
   <si>
     <t>1980 - Present</t>
+  </si>
+  <si>
+    <t>1983 to 2022</t>
+  </si>
+  <si>
+    <t>1970 - present</t>
   </si>
 </sst>
 </file>
@@ -1911,10 +1902,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
@@ -1923,10 +1914,10 @@
         <v>15</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1955,7 +1946,7 @@
         <v>131</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>132</v>
+        <v>305</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>37</v>
@@ -1969,25 +1960,25 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>99</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>131</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>37</v>
@@ -2001,13 +1992,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
@@ -2019,7 +2010,7 @@
         <v>24</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>37</v>
@@ -2033,10 +2024,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>129</v>
@@ -2045,13 +2036,13 @@
         <v>99</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>131</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>37</v>
@@ -2071,7 +2062,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>15</v>
@@ -2083,7 +2074,7 @@
         <v>21</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>37</v>
@@ -2101,7 +2092,7 @@
         <v>27</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>15</v>
@@ -2113,7 +2104,7 @@
         <v>21</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>37</v>
@@ -2127,13 +2118,13 @@
         <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>15</v>
@@ -2145,7 +2136,7 @@
         <v>21</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>36</v>
@@ -2157,13 +2148,13 @@
         <v>17</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>15</v>
@@ -2175,7 +2166,7 @@
         <v>21</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>36</v>
@@ -2189,13 +2180,13 @@
         <v>17</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>15</v>
@@ -2205,7 +2196,7 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>37</v>
@@ -2217,31 +2208,31 @@
         <v>17</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>36</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="31.5" x14ac:dyDescent="0.35">
@@ -2249,23 +2240,23 @@
         <v>17</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="9" t="s">
-        <v>292</v>
+        <v>100</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>37</v>
@@ -2277,23 +2268,23 @@
         <v>17</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="9" t="s">
-        <v>292</v>
+        <v>100</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J26" s="9" t="s">
         <v>37</v>
@@ -2305,23 +2296,23 @@
         <v>17</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>133</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>134</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9" t="s">
-        <v>300</v>
+        <v>99</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>37</v>
@@ -2340,16 +2331,16 @@
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>300</v>
+        <v>99</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>37</v>
@@ -2361,23 +2352,23 @@
         <v>17</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9" t="s">
-        <v>300</v>
+        <v>99</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="J29" s="9" t="s">
         <v>37</v>
@@ -2389,23 +2380,23 @@
         <v>17</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="J30" s="9" t="s">
         <v>37</v>
@@ -2417,23 +2408,23 @@
         <v>17</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="J31" s="9" t="s">
         <v>37</v>
@@ -2445,25 +2436,25 @@
         <v>33</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>24</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J32" s="9" t="s">
         <v>37</v>
@@ -2477,10 +2468,10 @@
         <v>33</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>12</v>
@@ -2489,19 +2480,19 @@
         <v>15</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>24</v>
       </c>
       <c r="I33" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="K33" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -2509,13 +2500,13 @@
         <v>33</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>15</v>
@@ -2527,13 +2518,13 @@
         <v>24</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J34" s="9" t="s">
         <v>36</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="2:11" ht="29" x14ac:dyDescent="0.35">
@@ -2541,10 +2532,10 @@
         <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>12</v>
@@ -2559,7 +2550,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2575,19 +2566,19 @@
         <v>27</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>37</v>
@@ -2621,19 +2612,19 @@
         <v>70</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H38" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J38" s="9" t="s">
         <v>115</v>
@@ -2647,25 +2638,25 @@
         <v>19</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>71</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J39" s="9" t="s">
         <v>110</v>
@@ -2679,25 +2670,25 @@
         <v>19</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>72</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>110</v>
@@ -2711,25 +2702,25 @@
         <v>19</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>73</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J41" s="9" t="s">
         <v>118</v>
@@ -2743,25 +2734,25 @@
         <v>19</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>74</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>115</v>
@@ -2775,25 +2766,25 @@
         <v>19</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H43" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>115</v>
@@ -2805,25 +2796,25 @@
         <v>19</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>75</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>119</v>
@@ -2837,25 +2828,25 @@
         <v>19</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>76</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>115</v>
@@ -2869,25 +2860,25 @@
         <v>19</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J46" s="9" t="s">
         <v>115</v>
@@ -2901,25 +2892,25 @@
         <v>19</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>78</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>115</v>
@@ -2933,25 +2924,25 @@
         <v>19</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>79</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H48" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J48" s="9" t="s">
         <v>111</v>
@@ -2971,19 +2962,19 @@
         <v>81</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>110</v>
@@ -2997,25 +2988,25 @@
         <v>19</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>82</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H50" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J50" s="9" t="s">
         <v>110</v>
@@ -3029,25 +3020,25 @@
         <v>19</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>83</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F51" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H51" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J51" s="9" t="s">
         <v>115</v>
@@ -3061,25 +3052,25 @@
         <v>19</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>84</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J52" s="9" t="s">
         <v>110</v>
@@ -3093,25 +3084,25 @@
         <v>19</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>85</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H53" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J53" s="9" t="s">
         <v>110</v>
@@ -3125,25 +3116,25 @@
         <v>19</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J54" s="9" t="s">
         <v>115</v>
@@ -3155,25 +3146,25 @@
         <v>19</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>116</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H55" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J55" s="9" t="s">
         <v>115</v>
@@ -3193,19 +3184,19 @@
         <v>86</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>112</v>
@@ -3225,19 +3216,19 @@
         <v>87</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>98</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H57" s="9" t="s">
         <v>102</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J57" s="9" t="s">
         <v>112</v>
@@ -3257,19 +3248,19 @@
         <v>88</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>101</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>117</v>
@@ -3289,7 +3280,7 @@
         <v>123</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>15</v>
@@ -3301,7 +3292,7 @@
         <v>105</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J59" s="9" t="s">
         <v>125</v>
@@ -3321,7 +3312,7 @@
         <v>89</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>99</v>
@@ -3333,7 +3324,7 @@
         <v>103</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J60" s="9" t="s">
         <v>115</v>
@@ -3353,19 +3344,19 @@
         <v>90</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>99</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H61" s="9" t="s">
         <v>104</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J61" s="9" t="s">
         <v>107</v>
@@ -3385,19 +3376,19 @@
         <v>91</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>99</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H62" s="9" t="s">
         <v>104</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J62" s="9" t="s">
         <v>107</v>
@@ -3417,19 +3408,19 @@
         <v>92</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>99</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H63" s="9" t="s">
         <v>104</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J63" s="9" t="s">
         <v>106</v>
@@ -3449,19 +3440,19 @@
         <v>93</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>99</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H64" s="9" t="s">
         <v>104</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J64" s="9" t="s">
         <v>107</v>
@@ -3481,7 +3472,7 @@
         <v>94</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>99</v>
@@ -3493,7 +3484,7 @@
         <v>104</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J65" s="9" t="s">
         <v>107</v>
@@ -3513,7 +3504,7 @@
         <v>95</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>100</v>
@@ -3525,7 +3516,7 @@
         <v>109</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J66" s="9" t="s">
         <v>113</v>
@@ -3545,19 +3536,19 @@
         <v>96</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>100</v>
       </c>
       <c r="G67" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="I67" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="I67" s="9" t="s">
-        <v>199</v>
       </c>
       <c r="J67" s="9" t="s">
         <v>110</v>
@@ -3577,19 +3568,19 @@
         <v>97</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>100</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J68" s="9" t="s">
         <v>114</v>
@@ -3609,7 +3600,7 @@
         <v>121</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F69" s="20" t="s">
         <v>100</v>
@@ -3621,7 +3612,7 @@
         <v>109</v>
       </c>
       <c r="I69" s="20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J69" s="20" t="s">
         <v>113</v>
@@ -3635,25 +3626,25 @@
         <v>16</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D70" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="H70" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F70" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="H70" s="9" t="s">
-        <v>206</v>
-      </c>
       <c r="I70" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J70" s="9" t="s">
         <v>37</v>
@@ -3667,25 +3658,25 @@
         <v>16</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J71" s="9" t="s">
         <v>37</v>
@@ -3705,7 +3696,7 @@
         <v>27</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>15</v>
@@ -3714,10 +3705,10 @@
         <v>20</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J72" s="9"/>
       <c r="K72" s="12" t="s">
@@ -3735,7 +3726,7 @@
         <v>29</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>15</v>
@@ -3747,7 +3738,7 @@
         <v>24</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J73" s="9"/>
       <c r="K73" s="12" t="s">
@@ -3759,13 +3750,13 @@
         <v>16</v>
       </c>
       <c r="C74" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="D74" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>215</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>15</v>
@@ -3774,10 +3765,10 @@
         <v>20</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J74" s="24" t="s">
         <v>36</v>
@@ -3797,19 +3788,19 @@
         <v>28</v>
       </c>
       <c r="E75" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H75" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="F75" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G75" s="9" t="s">
+      <c r="I75" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="H75" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="I75" s="9" t="s">
-        <v>220</v>
       </c>
       <c r="J75" s="9"/>
       <c r="K75" s="12" t="s">
@@ -3821,25 +3812,25 @@
         <v>16</v>
       </c>
       <c r="C76" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D76" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D76" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="E76" s="25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>99</v>
       </c>
       <c r="G76" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="I76" s="25" t="s">
         <v>222</v>
-      </c>
-      <c r="H76" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="I76" s="25" t="s">
-        <v>224</v>
       </c>
       <c r="J76" s="9" t="s">
         <v>37</v>
@@ -3853,25 +3844,25 @@
         <v>16</v>
       </c>
       <c r="C77" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D77" s="17" t="s">
+      <c r="F77" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="G77" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="H77" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="G77" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="H77" s="9" t="s">
-        <v>230</v>
-      </c>
       <c r="I77" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J77" s="24" t="s">
         <v>36</v>
@@ -3885,25 +3876,25 @@
         <v>16</v>
       </c>
       <c r="C78" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E78" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D78" s="10" t="s">
+      <c r="F78" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="H78" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="F78" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G78" s="9" t="s">
+      <c r="I78" s="9" t="s">
         <v>234</v>
-      </c>
-      <c r="H78" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="I78" s="9" t="s">
-        <v>236</v>
       </c>
       <c r="J78" s="9" t="s">
         <v>37</v>
@@ -3917,10 +3908,10 @@
         <v>16</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9" t="s">
@@ -3930,7 +3921,7 @@
         <v>47</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I79" s="9"/>
       <c r="J79" s="9" t="s">
@@ -3945,13 +3936,13 @@
         <v>16</v>
       </c>
       <c r="C80" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E80" s="9" t="s">
         <v>240</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>242</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>15</v>
@@ -3960,10 +3951,10 @@
         <v>47</v>
       </c>
       <c r="H80" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J80" s="9" t="s">
         <v>37</v>
@@ -3983,19 +3974,19 @@
         <v>31</v>
       </c>
       <c r="E81" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="H81" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="F81" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="H81" s="9" t="s">
-        <v>245</v>
-      </c>
       <c r="I81" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J81" s="9" t="s">
         <v>37</v>
@@ -4015,7 +4006,7 @@
         <v>32</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>15</v>
@@ -4024,10 +4015,10 @@
         <v>47</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J82" s="9" t="s">
         <v>37</v>
@@ -4041,13 +4032,13 @@
         <v>16</v>
       </c>
       <c r="C83" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E83" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>248</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>15</v>
@@ -4056,10 +4047,10 @@
         <v>47</v>
       </c>
       <c r="H83" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J83" s="9" t="s">
         <v>37</v>
@@ -4073,25 +4064,25 @@
         <v>16</v>
       </c>
       <c r="C84" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="D84" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G84" s="9" t="s">
-        <v>252</v>
-      </c>
       <c r="H84" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J84" s="9" t="s">
         <v>37</v>
@@ -4105,25 +4096,25 @@
         <v>16</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F85" s="9" t="s">
         <v>46</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I85" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J85" s="9" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
update presentations for tomorrow
</commit_message>
<xml_diff>
--- a/planning/Ageing-workshop-regional-homework-all-regions.xlsx
+++ b/planning/Ageing-workshop-regional-homework-all-regions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54689889-E98A-414B-910A-0FDD216A215E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96356A71-BD5F-4B3C-9624-E605185CA4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="312">
   <si>
     <t>Region</t>
   </si>
@@ -657,18 +657,12 @@
     <t>Research gillnet program, commercial samples, acoustic survey, annual trawl survey</t>
   </si>
   <si>
-    <t>NAFO 2J3KL,3NO,3Ps</t>
-  </si>
-  <si>
     <t xml:space="preserve">Crack and burn method, without burning (grinding if necessary) </t>
   </si>
   <si>
     <t>1950s to 2022</t>
   </si>
   <si>
-    <t>NAFO 3LNO, 3Ps, 2HJ3K</t>
-  </si>
-  <si>
     <t>Greenland Halibut</t>
   </si>
   <si>
@@ -693,9 +687,6 @@
     <t>1984 to 2019</t>
   </si>
   <si>
-    <t>NAFO 2HJ, 3KLMNO, 3ps, 4R</t>
-  </si>
-  <si>
     <t>Samples collected annually at Counting Fences and Fishways</t>
   </si>
   <si>
@@ -756,18 +747,12 @@
     <t>Sebastes spp.</t>
   </si>
   <si>
-    <t>NAFO 3LN, 3O, 2HJ3K</t>
-  </si>
-  <si>
     <t>NAFO 3LNO</t>
   </si>
   <si>
     <t>Annual trawl survey, at sea observers</t>
   </si>
   <si>
-    <t>Currently being collected and not red</t>
-  </si>
-  <si>
     <t>Atlantic Halibut</t>
   </si>
   <si>
@@ -864,30 +849,18 @@
     <t>Pacific Ocean Perch</t>
   </si>
   <si>
-    <t>5Z</t>
-  </si>
-  <si>
-    <t>4X</t>
-  </si>
-  <si>
     <t>Silver Hake</t>
   </si>
   <si>
     <t>Brosme brosme</t>
   </si>
   <si>
-    <t>4VWX</t>
-  </si>
-  <si>
     <t>1975 - present</t>
   </si>
   <si>
     <t>Hippoglossus hippoglosus</t>
   </si>
   <si>
-    <t>3NOPs4VWX5Zc</t>
-  </si>
-  <si>
     <t>Annual trawl survey, port sampling, at-sea observers, Industry Survey</t>
   </si>
   <si>
@@ -955,6 +928,48 @@
   </si>
   <si>
     <t>1970 - present</t>
+  </si>
+  <si>
+    <t>Start.year</t>
+  </si>
+  <si>
+    <t>End.year</t>
+  </si>
+  <si>
+    <t>NAFO 3Ps</t>
+  </si>
+  <si>
+    <t>NAFO 2HJ3K</t>
+  </si>
+  <si>
+    <t>NAFO 3NO</t>
+  </si>
+  <si>
+    <t>NAFO 3LN</t>
+  </si>
+  <si>
+    <t>NAFO 3O</t>
+  </si>
+  <si>
+    <t>NAFO 2HJ</t>
+  </si>
+  <si>
+    <t>NAFO 3KLMNO</t>
+  </si>
+  <si>
+    <t>NAFO 3ps</t>
+  </si>
+  <si>
+    <t>NAFO 4R</t>
+  </si>
+  <si>
+    <t>NAFO 5Z</t>
+  </si>
+  <si>
+    <t>NAFO 4X</t>
+  </si>
+  <si>
+    <t>NAFO 4VWX</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1224,33 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1263,19 +1304,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}" name="Table2" displayName="Table2" ref="B4:K69" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B4:K69" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1D9501B6-DF5E-4720-AD38-3FC53A5D3D5A}" name="Region" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{66C9233C-1717-4818-BD53-313537655389}" name="Species common name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{01FC48DD-5EDB-4D9B-8B4C-1F2E7A09D80E}" name="Species scientific name" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{9451EB80-E11C-4CCA-9087-FFE6D37C1345}" name="Stock area" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{DE2311AB-2B63-4FF4-8563-797A31472E6A}" name="Ageing structure" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{885148E1-C8BF-450C-8C44-7FC16D41E4FE}" name="Source(s) of ageing structures" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{1AD88BE3-1DA8-4D4F-8AC1-C881977CB5AF}" name="Preparation method" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{8384E904-7FFD-45BB-83B0-9CEFD2571836}" name="Years collected" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{3D42B2E0-7DD8-452F-9B97-D1252951BE09}" name="Age validation study" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{519A576D-E865-420A-A674-ECFFC4F66206}" name="Reference collection" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}" name="Table2" displayName="Table2" ref="B4:M69" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="B4:M69" xr:uid="{250A7792-A5E7-4986-923C-34151842E959}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{1D9501B6-DF5E-4720-AD38-3FC53A5D3D5A}" name="Region" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{66C9233C-1717-4818-BD53-313537655389}" name="Species common name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{01FC48DD-5EDB-4D9B-8B4C-1F2E7A09D80E}" name="Species scientific name" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{9451EB80-E11C-4CCA-9087-FFE6D37C1345}" name="Stock area" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DE2311AB-2B63-4FF4-8563-797A31472E6A}" name="Ageing structure" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{885148E1-C8BF-450C-8C44-7FC16D41E4FE}" name="Source(s) of ageing structures" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1AD88BE3-1DA8-4D4F-8AC1-C881977CB5AF}" name="Preparation method" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{8384E904-7FFD-45BB-83B0-9CEFD2571836}" name="Years collected" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{10990ED2-25B1-4D36-8A88-64E2CB420F6B}" name="Start.year" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{41F1614C-29CC-4EAD-9B2C-F66371F45F4A}" name="End.year" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{3D42B2E0-7DD8-452F-9B97-D1252951BE09}" name="Age validation study" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{519A576D-E865-420A-A674-ECFFC4F66206}" name="Reference collection" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1544,7 +1587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
@@ -1557,27 +1600,27 @@
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.81640625" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
-    <col min="10" max="10" width="24.453125" customWidth="1"/>
-    <col min="11" max="11" width="38.1796875" customWidth="1"/>
+    <col min="9" max="11" width="16.453125" customWidth="1"/>
+    <col min="12" max="12" width="24.453125" customWidth="1"/>
+    <col min="13" max="13" width="38.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1603,13 +1646,19 @@
         <v>3</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1634,14 +1683,20 @@
       <c r="I5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="2">
+        <v>1971</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1666,14 +1721,20 @@
       <c r="I6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="2">
+        <v>1971</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1698,14 +1759,20 @@
       <c r="I7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="2">
+        <v>1971</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1730,14 +1797,20 @@
       <c r="I8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="2">
+        <v>1971</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1762,14 +1835,20 @@
       <c r="I9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="2">
+        <v>1971</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1794,14 +1873,20 @@
       <c r="I10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="2">
+        <v>1971</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1826,14 +1911,20 @@
       <c r="I11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="2">
+        <v>2004</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2007</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1858,14 +1949,20 @@
       <c r="I12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="2">
+        <v>2004</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2017</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1890,14 +1987,20 @@
       <c r="I13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="2">
+        <v>2004</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2013</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1919,11 +2022,19 @@
       <c r="H14" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I14" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1965</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
@@ -1946,16 +2057,22 @@
         <v>131</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="J15" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1983</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1980,14 +2097,20 @@
       <c r="I16" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="2">
+        <v>1973</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
@@ -2012,14 +2135,20 @@
       <c r="I17" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="2">
+        <v>2021</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -2044,14 +2173,20 @@
       <c r="I18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="2">
+        <v>1995</v>
+      </c>
+      <c r="K18" s="2">
+        <v>2022</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2062,7 +2197,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>276</v>
+        <v>309</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>15</v>
@@ -2074,14 +2209,20 @@
         <v>21</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="J19" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="J19" s="9">
+        <v>1970</v>
+      </c>
+      <c r="K19" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="M19" s="12"/>
+    </row>
+    <row r="20" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
@@ -2092,7 +2233,7 @@
         <v>27</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>277</v>
+        <v>310</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>15</v>
@@ -2104,27 +2245,33 @@
         <v>21</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="J20" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="J20" s="9">
+        <v>1970</v>
+      </c>
+      <c r="K20" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="M20" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>276</v>
+        <v>309</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>15</v>
@@ -2136,25 +2283,31 @@
         <v>21</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="J21" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="J21" s="9">
+        <v>1970</v>
+      </c>
+      <c r="K21" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L21" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K21" s="12"/>
-    </row>
-    <row r="22" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="M21" s="12"/>
+    </row>
+    <row r="22" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>277</v>
+        <v>310</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>15</v>
@@ -2166,27 +2319,33 @@
         <v>21</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="J22" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="J22" s="9">
+        <v>1970</v>
+      </c>
+      <c r="K22" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="M22" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>15</v>
@@ -2196,102 +2355,118 @@
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="J23" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J23" s="9">
+        <v>1975</v>
+      </c>
+      <c r="K23" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="12"/>
-    </row>
-    <row r="24" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>283</v>
+        <v>241</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="J24" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="J24" s="9">
+        <v>1995</v>
+      </c>
+      <c r="K24" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K24" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="M24" s="12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="9" t="s">
         <v>100</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="J25" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="12"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M25" s="12"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="9" t="s">
         <v>100</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="J26" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="12"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M26" s="12"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
@@ -2306,20 +2481,26 @@
         <v>99</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="J27" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="J27" s="9">
+        <v>1950</v>
+      </c>
+      <c r="K27" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="12"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M27" s="12"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>17</v>
       </c>
@@ -2334,20 +2515,26 @@
         <v>99</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="J28" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="J28" s="9">
+        <v>1970</v>
+      </c>
+      <c r="K28" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="12"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M28" s="12"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
@@ -2362,20 +2549,26 @@
         <v>99</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="J29" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="J29" s="9">
+        <v>1970</v>
+      </c>
+      <c r="K29" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="12"/>
-    </row>
-    <row r="30" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="M29" s="12"/>
+    </row>
+    <row r="30" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
@@ -2387,51 +2580,63 @@
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="J30" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J30" s="9">
+        <v>1980</v>
+      </c>
+      <c r="K30" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="12"/>
-    </row>
-    <row r="31" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="M30" s="12"/>
+    </row>
+    <row r="31" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>21</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="J31" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="J31" s="9">
+        <v>1980</v>
+      </c>
+      <c r="K31" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K31" s="12"/>
-    </row>
-    <row r="32" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="M31" s="12"/>
+    </row>
+    <row r="32" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
@@ -2456,14 +2661,18 @@
       <c r="I32" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="J32" s="9" t="s">
+      <c r="J32" s="9"/>
+      <c r="K32" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L32" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="M32" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
@@ -2488,19 +2697,25 @@
       <c r="I33" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="J33" s="9" t="s">
+      <c r="J33" s="9">
+        <v>1984</v>
+      </c>
+      <c r="K33" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L33" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="M33" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>157</v>
@@ -2520,22 +2735,28 @@
       <c r="I34" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="J34" s="9" t="s">
+      <c r="J34" s="9">
+        <v>1973</v>
+      </c>
+      <c r="K34" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L34" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="M34" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>12</v>
@@ -2550,12 +2771,18 @@
         <v>24</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+        <v>253</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1990</v>
+      </c>
+      <c r="K35" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
@@ -2566,28 +2793,34 @@
         <v>27</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="J36" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1974</v>
+      </c>
+      <c r="K36" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>18</v>
       </c>
@@ -2600,8 +2833,10 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
@@ -2626,19 +2861,25 @@
       <c r="I38" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="J38" s="9">
+        <v>1980</v>
+      </c>
+      <c r="K38" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L38" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K38" s="12" t="s">
+      <c r="M38" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>71</v>
@@ -2658,19 +2899,25 @@
       <c r="I39" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J39" s="9" t="s">
+      <c r="J39" s="9">
+        <v>1964</v>
+      </c>
+      <c r="K39" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L39" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K39" s="12" t="s">
+      <c r="M39" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>72</v>
@@ -2690,19 +2937,25 @@
       <c r="I40" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="9">
+        <v>1979</v>
+      </c>
+      <c r="K40" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L40" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K40" s="12" t="s">
+      <c r="M40" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>73</v>
@@ -2722,19 +2975,25 @@
       <c r="I41" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="J41" s="9" t="s">
+      <c r="J41" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K41" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L41" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="K41" s="12" t="s">
+      <c r="M41" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>74</v>
@@ -2754,19 +3013,25 @@
       <c r="I42" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="J42" s="9">
+        <v>1973</v>
+      </c>
+      <c r="K42" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L42" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K42" s="12" t="s">
+      <c r="M42" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>166</v>
@@ -2786,17 +3051,23 @@
       <c r="I43" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="J43" s="9">
+        <v>1986</v>
+      </c>
+      <c r="K43" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L43" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K43" s="12"/>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M43" s="12"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>75</v>
@@ -2816,19 +3087,25 @@
       <c r="I44" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="J44" s="9">
+        <v>1980</v>
+      </c>
+      <c r="K44" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L44" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="M44" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>76</v>
@@ -2848,19 +3125,25 @@
       <c r="I45" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="J45" s="9" t="s">
+      <c r="J45" s="9">
+        <v>1973</v>
+      </c>
+      <c r="K45" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L45" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K45" s="12" t="s">
+      <c r="M45" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>77</v>
@@ -2880,19 +3163,25 @@
       <c r="I46" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="J46" s="9" t="s">
+      <c r="J46" s="9">
+        <v>1984</v>
+      </c>
+      <c r="K46" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L46" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K46" s="12" t="s">
+      <c r="M46" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>78</v>
@@ -2912,19 +3201,25 @@
       <c r="I47" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="J47" s="9">
+        <v>1979</v>
+      </c>
+      <c r="K47" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L47" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K47" s="12" t="s">
+      <c r="M47" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>79</v>
@@ -2944,14 +3239,20 @@
       <c r="I48" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="J48" s="9">
+        <v>1977</v>
+      </c>
+      <c r="K48" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L48" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="K48" s="12" t="s">
+      <c r="M48" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
         <v>19</v>
       </c>
@@ -2976,19 +3277,25 @@
       <c r="I49" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="J49" s="9" t="s">
+      <c r="J49" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K49" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L49" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="M49" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>82</v>
@@ -3008,19 +3315,25 @@
       <c r="I50" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="J50" s="9" t="s">
+      <c r="J50" s="9">
+        <v>1973</v>
+      </c>
+      <c r="K50" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L50" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="M50" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>83</v>
@@ -3040,19 +3353,25 @@
       <c r="I51" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="J51" s="9" t="s">
+      <c r="J51" s="9">
+        <v>1977</v>
+      </c>
+      <c r="K51" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L51" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K51" s="12" t="s">
+      <c r="M51" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D52" s="15" t="s">
         <v>84</v>
@@ -3072,19 +3391,25 @@
       <c r="I52" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="J52" s="9" t="s">
+      <c r="J52" s="9">
+        <v>1977</v>
+      </c>
+      <c r="K52" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L52" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K52" s="12" t="s">
+      <c r="M52" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>85</v>
@@ -3104,19 +3429,25 @@
       <c r="I53" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J53" s="9" t="s">
+      <c r="J53" s="9">
+        <v>1979</v>
+      </c>
+      <c r="K53" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L53" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K53" s="12" t="s">
+      <c r="M53" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>170</v>
@@ -3136,17 +3467,23 @@
       <c r="I54" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J54" s="9" t="s">
+      <c r="J54" s="9">
+        <v>1979</v>
+      </c>
+      <c r="K54" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L54" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K54" s="12"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="M54" s="12"/>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>116</v>
@@ -3166,14 +3503,20 @@
       <c r="I55" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="J55" s="9" t="s">
+      <c r="J55" s="9">
+        <v>1966</v>
+      </c>
+      <c r="K55" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L55" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K55" s="12" t="s">
+      <c r="M55" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B56" s="2" t="s">
         <v>19</v>
       </c>
@@ -3198,14 +3541,20 @@
       <c r="I56" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="J56" s="9" t="s">
+      <c r="J56" s="9">
+        <v>1965</v>
+      </c>
+      <c r="K56" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L56" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="K56" s="12" t="s">
+      <c r="M56" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
         <v>19</v>
       </c>
@@ -3230,14 +3579,20 @@
       <c r="I57" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="J57" s="9" t="s">
+      <c r="J57" s="9">
+        <v>1965</v>
+      </c>
+      <c r="K57" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L57" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="K57" s="12" t="s">
+      <c r="M57" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
         <v>19</v>
       </c>
@@ -3262,14 +3617,20 @@
       <c r="I58" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="J58" s="9" t="s">
+      <c r="J58" s="9">
+        <v>1985</v>
+      </c>
+      <c r="K58" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L58" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="K58" s="12" t="s">
+      <c r="M58" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B59" s="2" t="s">
         <v>19</v>
       </c>
@@ -3294,14 +3655,20 @@
       <c r="I59" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="J59" s="9" t="s">
+      <c r="J59" s="9">
+        <v>2015</v>
+      </c>
+      <c r="K59" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L59" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="K59" s="12" t="s">
+      <c r="M59" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
         <v>19</v>
       </c>
@@ -3326,14 +3693,20 @@
       <c r="I60" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="J60" s="9" t="s">
+      <c r="J60" s="9">
+        <v>1992</v>
+      </c>
+      <c r="K60" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L60" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="K60" s="12" t="s">
+      <c r="M60" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B61" s="2" t="s">
         <v>19</v>
       </c>
@@ -3358,14 +3731,20 @@
       <c r="I61" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="J61" s="9" t="s">
+      <c r="J61" s="9">
+        <v>1900</v>
+      </c>
+      <c r="K61" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L61" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K61" s="12" t="s">
+      <c r="M61" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B62" s="2" t="s">
         <v>19</v>
       </c>
@@ -3390,14 +3769,20 @@
       <c r="I62" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="J62" s="9" t="s">
+      <c r="J62" s="9">
+        <v>1901</v>
+      </c>
+      <c r="K62" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L62" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K62" s="12" t="s">
+      <c r="M62" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B63" s="2" t="s">
         <v>19</v>
       </c>
@@ -3422,14 +3807,20 @@
       <c r="I63" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="J63" s="9" t="s">
+      <c r="J63" s="9">
+        <v>1902</v>
+      </c>
+      <c r="K63" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L63" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="K63" s="12" t="s">
+      <c r="M63" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B64" s="2" t="s">
         <v>19</v>
       </c>
@@ -3454,14 +3845,20 @@
       <c r="I64" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="J64" s="9" t="s">
+      <c r="J64" s="9">
+        <v>1903</v>
+      </c>
+      <c r="K64" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L64" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K64" s="12" t="s">
+      <c r="M64" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="2" t="s">
         <v>19</v>
       </c>
@@ -3486,14 +3883,20 @@
       <c r="I65" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="J65" s="9" t="s">
+      <c r="J65" s="9">
+        <v>1904</v>
+      </c>
+      <c r="K65" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L65" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K65" s="12" t="s">
+      <c r="M65" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="2" t="s">
         <v>19</v>
       </c>
@@ -3518,14 +3921,20 @@
       <c r="I66" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="J66" s="9" t="s">
+      <c r="J66" s="9">
+        <v>2000</v>
+      </c>
+      <c r="K66" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L66" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="K66" s="12" t="s">
+      <c r="M66" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B67" s="2" t="s">
         <v>19</v>
       </c>
@@ -3550,14 +3959,20 @@
       <c r="I67" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="J67" s="9" t="s">
+      <c r="J67" s="9">
+        <v>2003</v>
+      </c>
+      <c r="K67" s="9">
+        <v>2020</v>
+      </c>
+      <c r="L67" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="K67" s="12" t="s">
+      <c r="M67" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B68" s="2" t="s">
         <v>19</v>
       </c>
@@ -3582,14 +3997,20 @@
       <c r="I68" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J68" s="9" t="s">
+      <c r="J68" s="9">
+        <v>1995</v>
+      </c>
+      <c r="K68" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L68" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="K68" s="12" t="s">
+      <c r="M68" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B69" s="2" t="s">
         <v>19</v>
       </c>
@@ -3614,14 +4035,20 @@
       <c r="I69" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="J69" s="20" t="s">
+      <c r="J69" s="20">
+        <v>2019</v>
+      </c>
+      <c r="K69" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L69" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="K69" s="22" t="s">
+      <c r="M69" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B70" s="27" t="s">
         <v>16</v>
       </c>
@@ -3646,14 +4073,20 @@
       <c r="I70" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="J70" s="9" t="s">
+      <c r="J70" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K70" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L70" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K70" s="12" t="s">
+      <c r="M70" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B71" s="27" t="s">
         <v>16</v>
       </c>
@@ -3678,14 +4111,20 @@
       <c r="I71" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="J71" s="9" t="s">
+      <c r="J71" s="9">
+        <v>1965</v>
+      </c>
+      <c r="K71" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L71" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K71" s="12" t="s">
+      <c r="M71" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B72" s="27" t="s">
         <v>16</v>
       </c>
@@ -3696,7 +4135,7 @@
         <v>27</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>15</v>
@@ -3705,28 +4144,32 @@
         <v>20</v>
       </c>
       <c r="H72" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I72" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="I72" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="J72" s="9"/>
-      <c r="K72" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J72" s="9">
+        <v>1950</v>
+      </c>
+      <c r="K72" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L72" s="9"/>
+      <c r="M72" s="12"/>
+    </row>
+    <row r="73" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B73" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>210</v>
+        <v>302</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>15</v>
@@ -3735,28 +4178,32 @@
         <v>20</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>24</v>
+        <v>207</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J73" s="9"/>
-      <c r="K73" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+      <c r="J73" s="9">
+        <v>1950</v>
+      </c>
+      <c r="K73" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L73" s="9"/>
+      <c r="M73" s="12"/>
+    </row>
+    <row r="74" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B74" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D74" s="23" t="s">
-        <v>212</v>
+        <v>38</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>213</v>
+        <v>300</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>15</v>
@@ -3765,370 +4212,920 @@
         <v>20</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J74" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="K74" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="J74" s="9">
+        <v>1950</v>
+      </c>
+      <c r="K74" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L74" s="9"/>
+      <c r="M74" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B75" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>216</v>
+        <v>20</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>217</v>
+        <v>24</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="J75" s="9"/>
-      <c r="K75" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="76" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+      <c r="J75" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K75" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L75" s="9"/>
+      <c r="M75" s="12"/>
+    </row>
+    <row r="76" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B76" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E76" s="25" t="s">
-        <v>219</v>
+        <v>29</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>300</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G76" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="H76" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="I76" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="J76" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K76" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="77" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J76" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K76" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L76" s="9"/>
+      <c r="M76" s="12"/>
+    </row>
+    <row r="77" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B77" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>224</v>
+        <v>6</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>225</v>
+        <v>301</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>226</v>
+        <v>15</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>227</v>
+        <v>20</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>228</v>
+        <v>24</v>
       </c>
       <c r="I77" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="J77" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="K77" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="J77" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K77" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L77" s="9"/>
+      <c r="M77" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B78" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>230</v>
+        <v>209</v>
+      </c>
+      <c r="D78" s="23" t="s">
+        <v>210</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>232</v>
+        <v>20</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="J78" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K78" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+      <c r="J78" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K78" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L78" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M78" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B79" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>235</v>
+        <v>7</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="E79" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="F79" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="H79" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="I79" s="9"/>
-      <c r="J79" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K79" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="80" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="J79" s="9">
+        <v>1984</v>
+      </c>
+      <c r="K79" s="9">
+        <v>2019</v>
+      </c>
+      <c r="L79" s="9"/>
+      <c r="M79" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B80" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>238</v>
+        <v>132</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>240</v>
+        <v>133</v>
+      </c>
+      <c r="E80" s="25" t="s">
+        <v>305</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G80" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H80" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="I80" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J80" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G80" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H80" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="I80" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="J80" s="25">
+        <v>1975</v>
+      </c>
+      <c r="K80" s="25">
+        <v>2023</v>
+      </c>
+      <c r="L80" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K80" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="M80" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B81" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>9</v>
+        <v>132</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>241</v>
+        <v>133</v>
+      </c>
+      <c r="E81" s="25" t="s">
+        <v>306</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G81" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="H81" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="I81" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J81" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G81" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H81" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="I81" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="J81" s="25">
+        <v>1975</v>
+      </c>
+      <c r="K81" s="25">
+        <v>2023</v>
+      </c>
+      <c r="L81" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K81" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="82" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="M81" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B82" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>207</v>
+        <v>133</v>
+      </c>
+      <c r="E82" s="25" t="s">
+        <v>307</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H82" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="I82" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J82" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G82" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H82" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="I82" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="J82" s="25">
+        <v>1975</v>
+      </c>
+      <c r="K82" s="25">
+        <v>2023</v>
+      </c>
+      <c r="L82" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K82" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="83" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="M82" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B83" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>244</v>
+        <v>132</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>246</v>
+        <v>133</v>
+      </c>
+      <c r="E83" s="25" t="s">
+        <v>308</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G83" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H83" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="I83" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J83" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G83" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="H83" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="I83" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="J83" s="25">
+        <v>1975</v>
+      </c>
+      <c r="K83" s="25">
+        <v>2023</v>
+      </c>
+      <c r="L83" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K83" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="M83" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B84" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="H84" s="9" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J84" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K84" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="85" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+      <c r="J84" s="9">
+        <v>1979</v>
+      </c>
+      <c r="K84" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L84" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="M84" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B85" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="E85" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="H85" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="I85" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="F85" s="9" t="s">
+      <c r="J85" s="9">
+        <v>2001</v>
+      </c>
+      <c r="K85" s="9">
+        <v>2006</v>
+      </c>
+      <c r="L85" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M85" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B86" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M86" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B87" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H87" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I87" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J87" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K87" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L87" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M87" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B88" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J88" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K88" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L88" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M88" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B89" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J89" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K89" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L89" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M89" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B90" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I90" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J90" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K90" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L90" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M90" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B91" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I91" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J91" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K91" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L91" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M91" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B92" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J92" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K92" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L92" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M92" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B93" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H93" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I93" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J93" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K93" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L93" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M93" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B94" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H94" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="I94" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J94" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K94" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L94" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M94" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B95" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="I95" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J95" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K95" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L95" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M95" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B96" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D96" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="H96" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="I96" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J96" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K96" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L96" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M96" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B97" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D97" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="H97" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="I97" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J97" s="9">
+        <v>1978</v>
+      </c>
+      <c r="K97" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L97" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M97" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B98" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="F98" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G85" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="H85" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="I85" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="J85" s="9" t="s">
+      <c r="G98" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="H98" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="I98" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="J98" s="9">
+        <v>2004</v>
+      </c>
+      <c r="K98" s="9">
+        <v>2022</v>
+      </c>
+      <c r="L98" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K85" s="12" t="s">
+      <c r="M98" s="12" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J7" r:id="rId1" xr:uid="{AE9870F2-46B7-4F0E-BEAD-2C74FAC27E5A}"/>
-    <hyperlink ref="J74" r:id="rId2" xr:uid="{192468E9-F3F8-48E1-A457-9E87E99A73CC}"/>
-    <hyperlink ref="J77" r:id="rId3" xr:uid="{9361AF13-362F-4D8A-9FCB-B8CB2E1CB121}"/>
+    <hyperlink ref="L7" r:id="rId1" xr:uid="{AE9870F2-46B7-4F0E-BEAD-2C74FAC27E5A}"/>
+    <hyperlink ref="L78" r:id="rId2" xr:uid="{192468E9-F3F8-48E1-A457-9E87E99A73CC}"/>
+    <hyperlink ref="L84" r:id="rId3" xr:uid="{9361AF13-362F-4D8A-9FCB-B8CB2E1CB121}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
add Day 1 edits from Jacob, and get ready for initial submission
</commit_message>
<xml_diff>
--- a/planning/Ageing-workshop-regional-homework-all-regions.xlsx
+++ b/planning/Ageing-workshop-regional-homework-all-regions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc-my.sharepoint.com/personal/daniel_ricard_dfo-mpo_gc_ca/Documents/Documents/GitHub/ageing-best-practices-2023/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958294BC-080D-45F6-A58C-69867F9750FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{958294BC-080D-45F6-A58C-69867F9750FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876E77F2-BFB1-4C52-B7B1-1336F3468897}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="4965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45120" yWindow="45" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="422">
   <si>
     <t>Region</t>
   </si>
@@ -435,9 +435,6 @@
     <t>SFA 18</t>
   </si>
   <si>
-    <t>2021-2022</t>
-  </si>
-  <si>
     <t>Striped Bass</t>
   </si>
   <si>
@@ -894,9 +891,6 @@
     <t>mounted in epoxy resin Whole Otolith</t>
   </si>
   <si>
-    <t>1954-2022</t>
-  </si>
-  <si>
     <t>Yes*</t>
   </si>
   <si>
@@ -1251,27 +1245,6 @@
     <t>SFA 16, 18</t>
   </si>
   <si>
-    <t>1970 - 2022</t>
-  </si>
-  <si>
-    <t>1975 - 2022</t>
-  </si>
-  <si>
-    <t>1995-2022</t>
-  </si>
-  <si>
-    <t>1950? - 2022</t>
-  </si>
-  <si>
-    <t>1970? - 2022</t>
-  </si>
-  <si>
-    <t>1980? - 2022</t>
-  </si>
-  <si>
-    <t>1980 - 2022</t>
-  </si>
-  <si>
     <t>1970s to 2022</t>
   </si>
   <si>
@@ -1312,6 +1285,21 @@
   </si>
   <si>
     <t>PMFC 3CD,4B,5ABCE</t>
+  </si>
+  <si>
+    <t>1970 to 2022</t>
+  </si>
+  <si>
+    <t>1954 to 2022</t>
+  </si>
+  <si>
+    <t>1975 to 2022</t>
+  </si>
+  <si>
+    <t>1980s to 2022</t>
+  </si>
+  <si>
+    <t>2021 and 2022</t>
   </si>
 </sst>
 </file>
@@ -2212,9 +2200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2238,12 +2224,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2251,13 +2237,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>38</v>
@@ -2266,7 +2252,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>31</v>
@@ -2278,10 +2264,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>281</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>37</v>
@@ -2290,7 +2276,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2304,7 +2290,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
@@ -2313,7 +2299,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>17</v>
@@ -2352,7 +2338,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>11</v>
@@ -2361,7 +2347,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>17</v>
@@ -2400,7 +2386,7 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
@@ -2409,7 +2395,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>17</v>
@@ -2448,7 +2434,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
@@ -2457,7 +2443,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>17</v>
@@ -2496,7 +2482,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>11</v>
@@ -2505,7 +2491,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>17</v>
@@ -2544,7 +2530,7 @@
         <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>12</v>
@@ -2553,7 +2539,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>17</v>
@@ -2592,7 +2578,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
@@ -2601,7 +2587,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>42</v>
@@ -2640,7 +2626,7 @@
         <v>47</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>11</v>
@@ -2649,7 +2635,7 @@
         <v>41</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>42</v>
@@ -2688,7 +2674,7 @@
         <v>48</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>11</v>
@@ -2697,7 +2683,7 @@
         <v>41</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>42</v>
@@ -2730,13 +2716,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>11</v>
@@ -2745,16 +2731,16 @@
         <v>13</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="K14" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L14" s="3">
         <v>1965</v>
@@ -2784,16 +2770,16 @@
         <v>123</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>124</v>
@@ -2802,7 +2788,7 @@
         <v>125</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L15" s="3">
         <v>1983</v>
@@ -2832,7 +2818,7 @@
         <v>127</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>128</v>
@@ -2841,7 +2827,7 @@
         <v>94</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>129</v>
@@ -2850,7 +2836,7 @@
         <v>125</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L16" s="3">
         <v>1973</v>
@@ -2880,7 +2866,7 @@
         <v>131</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>132</v>
@@ -2889,7 +2875,7 @@
         <v>13</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>124</v>
@@ -2898,7 +2884,7 @@
         <v>21</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>133</v>
+        <v>421</v>
       </c>
       <c r="L17" s="3">
         <v>2021</v>
@@ -2922,31 +2908,31 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>125</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L18" s="3">
         <v>1995</v>
@@ -2976,16 +2962,16 @@
         <v>24</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>17</v>
@@ -2994,7 +2980,7 @@
         <v>18</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="L19" s="9">
         <v>1970</v>
@@ -3022,16 +3008,16 @@
         <v>24</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>17</v>
@@ -3040,7 +3026,7 @@
         <v>18</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="L20" s="9">
         <v>1970</v>
@@ -3064,31 +3050,31 @@
         <v>15</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>139</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>286</v>
+        <v>418</v>
       </c>
       <c r="L21" s="12">
         <v>1954</v>
@@ -3097,7 +3083,7 @@
         <v>2022</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>19</v>
@@ -3112,22 +3098,22 @@
         <v>15</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>233</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>17</v>
@@ -3136,7 +3122,7 @@
         <v>18</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="L22" s="9">
         <v>1970</v>
@@ -3158,22 +3144,22 @@
         <v>15</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>233</v>
-      </c>
       <c r="E23" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>17</v>
@@ -3182,7 +3168,7 @@
         <v>18</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="L23" s="9">
         <v>1970</v>
@@ -3206,22 +3192,22 @@
         <v>15</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I24" s="14" t="s">
         <v>17</v>
@@ -3230,7 +3216,7 @@
         <v>18</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="L24" s="16">
         <v>1970</v>
@@ -3254,29 +3240,29 @@
         <v>15</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>261</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>17</v>
       </c>
       <c r="J25" s="17"/>
       <c r="K25" s="9" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="L25" s="9">
         <v>1975</v>
@@ -3298,31 +3284,31 @@
         <v>15</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J26" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>407</v>
+        <v>136</v>
       </c>
       <c r="L26" s="9">
         <v>1995</v>
@@ -3334,7 +3320,7 @@
         <v>33</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P26" s="3" t="str">
         <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
@@ -3346,29 +3332,29 @@
         <v>15</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>266</v>
-      </c>
       <c r="E27" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="9" t="s">
         <v>95</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I27" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="J27" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="J27" s="17" t="s">
+      <c r="K27" s="9" t="s">
         <v>268</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>269</v>
       </c>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
@@ -3386,29 +3372,29 @@
         <v>15</v>
       </c>
       <c r="C28" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>271</v>
-      </c>
       <c r="E28" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="9" t="s">
         <v>95</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I28" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="J28" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="J28" s="17" t="s">
-        <v>273</v>
-      </c>
       <c r="K28" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
@@ -3432,23 +3418,23 @@
         <v>127</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I29" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J29" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="J29" s="17" t="s">
-        <v>275</v>
-      </c>
       <c r="K29" s="9" t="s">
-        <v>408</v>
+        <v>196</v>
       </c>
       <c r="L29" s="9">
         <v>1950</v>
@@ -3476,23 +3462,23 @@
         <v>123</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H30" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="K30" s="9" t="s">
         <v>403</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>409</v>
       </c>
       <c r="L30" s="9">
         <v>1970</v>
@@ -3520,23 +3506,23 @@
         <v>131</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H31" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="K31" s="9" t="s">
         <v>403</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>409</v>
       </c>
       <c r="L31" s="9">
         <v>1970</v>
@@ -3558,29 +3544,29 @@
         <v>15</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>135</v>
-      </c>
       <c r="E32" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J32" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="L32" s="9">
         <v>1980</v>
@@ -3602,29 +3588,29 @@
         <v>15</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>278</v>
-      </c>
       <c r="E33" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>411</v>
+        <v>154</v>
       </c>
       <c r="L33" s="9">
         <v>1980</v>
@@ -3646,31 +3632,31 @@
         <v>30</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>139</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>21</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L34" s="9">
         <v>1965</v>
@@ -3694,13 +3680,13 @@
         <v>30</v>
       </c>
       <c r="C35" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>146</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>12</v>
@@ -3709,16 +3695,16 @@
         <v>13</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>21</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L35" s="9">
         <v>1984</v>
@@ -3727,10 +3713,10 @@
         <v>2022</v>
       </c>
       <c r="N35" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="O35" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="O35" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="P35" s="3" t="str">
         <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
@@ -3742,22 +3728,22 @@
         <v>30</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>17</v>
@@ -3766,7 +3752,7 @@
         <v>21</v>
       </c>
       <c r="K36" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L36" s="9">
         <v>1973</v>
@@ -3778,7 +3764,7 @@
         <v>33</v>
       </c>
       <c r="O36" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P36" s="3" t="str">
         <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
@@ -3790,13 +3776,13 @@
         <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>229</v>
-      </c>
       <c r="E37" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>12</v>
@@ -3805,7 +3791,7 @@
         <v>13</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>17</v>
@@ -3814,7 +3800,7 @@
         <v>21</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L37" s="3">
         <v>1990</v>
@@ -3840,25 +3826,25 @@
         <v>24</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I38" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="J38" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="J38" s="21" t="s">
+      <c r="K38" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="L38" s="3">
         <v>1974</v>
@@ -3888,25 +3874,25 @@
         <v>65</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J39" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L39" s="9">
         <v>1980</v>
@@ -3930,31 +3916,31 @@
         <v>16</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D40" s="23" t="s">
         <v>66</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L40" s="9">
         <v>1964</v>
@@ -3978,31 +3964,31 @@
         <v>16</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>67</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J41" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L41" s="9">
         <v>1979</v>
@@ -4026,31 +4012,31 @@
         <v>16</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>68</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J42" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L42" s="9">
         <v>1978</v>
@@ -4074,31 +4060,31 @@
         <v>16</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>69</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L43" s="9">
         <v>1973</v>
@@ -4122,31 +4108,31 @@
         <v>16</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L44" s="9">
         <v>1986</v>
@@ -4168,31 +4154,31 @@
         <v>16</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D45" s="24" t="s">
         <v>70</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J45" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L45" s="9">
         <v>1980</v>
@@ -4216,31 +4202,31 @@
         <v>16</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D46" s="24" t="s">
         <v>71</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J46" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L46" s="9">
         <v>1973</v>
@@ -4264,31 +4250,31 @@
         <v>16</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D47" s="24" t="s">
         <v>72</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L47" s="9">
         <v>1984</v>
@@ -4312,31 +4298,31 @@
         <v>16</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D48" s="24" t="s">
         <v>73</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J48" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L48" s="9">
         <v>1979</v>
@@ -4360,31 +4346,31 @@
         <v>16</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D49" s="24" t="s">
         <v>74</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L49" s="9">
         <v>1977</v>
@@ -4414,25 +4400,25 @@
         <v>76</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J50" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L50" s="9">
         <v>1978</v>
@@ -4456,31 +4442,31 @@
         <v>16</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>77</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J51" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L51" s="9">
         <v>1973</v>
@@ -4504,31 +4490,31 @@
         <v>16</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D52" s="24" t="s">
         <v>78</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J52" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L52" s="9">
         <v>1977</v>
@@ -4552,31 +4538,31 @@
         <v>16</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>79</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J53" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L53" s="9">
         <v>1977</v>
@@ -4600,31 +4586,31 @@
         <v>16</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D54" s="24" t="s">
         <v>80</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J54" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L54" s="9">
         <v>1979</v>
@@ -4648,31 +4634,31 @@
         <v>16</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J55" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L55" s="9">
         <v>1979</v>
@@ -4694,31 +4680,31 @@
         <v>16</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D56" s="26" t="s">
         <v>111</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L56" s="9">
         <v>1966</v>
@@ -4748,25 +4734,25 @@
         <v>81</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="G57" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J57" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L57" s="9">
         <v>1965</v>
@@ -4796,25 +4782,25 @@
         <v>82</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>93</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>97</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L58" s="9">
         <v>1965</v>
@@ -4844,25 +4830,25 @@
         <v>83</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J59" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L59" s="9">
         <v>1985</v>
@@ -4892,16 +4878,16 @@
         <v>118</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I60" s="9" t="s">
         <v>42</v>
@@ -4910,7 +4896,7 @@
         <v>100</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L60" s="9">
         <v>2015</v>
@@ -4940,16 +4926,16 @@
         <v>84</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G61" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I61" s="9" t="s">
         <v>17</v>
@@ -4958,7 +4944,7 @@
         <v>98</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L61" s="9">
         <v>1992</v>
@@ -4988,25 +4974,25 @@
         <v>85</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J62" s="9" t="s">
         <v>99</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L62" s="9">
         <v>1900</v>
@@ -5036,25 +5022,25 @@
         <v>86</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G63" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J63" s="9" t="s">
         <v>99</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L63" s="9">
         <v>1901</v>
@@ -5084,25 +5070,25 @@
         <v>87</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G64" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J64" s="9" t="s">
         <v>99</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L64" s="9">
         <v>1902</v>
@@ -5132,25 +5118,25 @@
         <v>88</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G65" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J65" s="9" t="s">
         <v>99</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L65" s="9">
         <v>1903</v>
@@ -5180,16 +5166,16 @@
         <v>89</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G66" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I66" s="9" t="s">
         <v>17</v>
@@ -5198,7 +5184,7 @@
         <v>99</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L66" s="9">
         <v>1904</v>
@@ -5228,16 +5214,16 @@
         <v>90</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G67" s="9" t="s">
         <v>95</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I67" s="9" t="s">
         <v>121</v>
@@ -5246,7 +5232,7 @@
         <v>104</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L67" s="9">
         <v>2000</v>
@@ -5276,25 +5262,25 @@
         <v>91</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G68" s="9" t="s">
         <v>95</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I68" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="J68" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="9" t="s">
+      <c r="K68" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="K68" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="L68" s="9">
         <v>2003</v>
@@ -5324,25 +5310,25 @@
         <v>92</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G69" s="9" t="s">
         <v>95</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L69" s="9">
         <v>1995</v>
@@ -5372,16 +5358,16 @@
         <v>116</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F70" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G70" s="29" t="s">
         <v>95</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I70" s="29" t="s">
         <v>117</v>
@@ -5390,7 +5376,7 @@
         <v>104</v>
       </c>
       <c r="K70" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L70" s="29">
         <v>2019</v>
@@ -5414,31 +5400,31 @@
         <v>14</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D71" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F71" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="G71" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I71" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="J71" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="J71" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="K71" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L71" s="9">
         <v>1978</v>
@@ -5462,31 +5448,31 @@
         <v>14</v>
       </c>
       <c r="C72" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D72" s="10" t="s">
-        <v>139</v>
-      </c>
       <c r="E72" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G72" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L72" s="9">
         <v>1965</v>
@@ -5516,25 +5502,25 @@
         <v>24</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="G73" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I73" s="9" t="s">
         <v>17</v>
       </c>
       <c r="J73" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="K73" s="9" t="s">
         <v>196</v>
-      </c>
-      <c r="K73" s="9" t="s">
-        <v>197</v>
       </c>
       <c r="L73" s="9">
         <v>1950</v>
@@ -5544,7 +5530,7 @@
       </c>
       <c r="N73" s="9"/>
       <c r="O73" s="11" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="P73" s="3" t="str">
         <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
@@ -5562,16 +5548,16 @@
         <v>26</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I74" s="9" t="s">
         <v>17</v>
@@ -5580,7 +5566,7 @@
         <v>21</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L74" s="9">
         <v>1978</v>
@@ -5590,7 +5576,7 @@
       </c>
       <c r="N74" s="9"/>
       <c r="O74" s="11" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="P74" s="3" t="str">
         <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
@@ -5602,31 +5588,31 @@
         <v>14</v>
       </c>
       <c r="C75" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D75" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="D75" s="33" t="s">
+      <c r="E75" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F75" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>200</v>
       </c>
       <c r="G75" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I75" s="9" t="s">
         <v>17</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L75" s="9">
         <v>1978</v>
@@ -5656,25 +5642,25 @@
         <v>25</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G76" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I76" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J76" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="J76" s="9" t="s">
+      <c r="K76" s="9" t="s">
         <v>204</v>
-      </c>
-      <c r="K76" s="9" t="s">
-        <v>205</v>
       </c>
       <c r="L76" s="9">
         <v>1984</v>
@@ -5702,25 +5688,25 @@
         <v>127</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F77" s="35" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="G77" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I77" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="J77" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="J77" s="35" t="s">
+      <c r="K77" s="35" t="s">
         <v>207</v>
-      </c>
-      <c r="K77" s="35" t="s">
-        <v>208</v>
       </c>
       <c r="L77" s="35">
         <v>1975</v>
@@ -5744,31 +5730,31 @@
         <v>14</v>
       </c>
       <c r="C78" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D78" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="D78" s="26" t="s">
+      <c r="E78" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="E78" s="26" t="s">
-        <v>397</v>
-      </c>
-      <c r="F78" s="9" t="s">
+      <c r="G78" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="G78" s="9" t="s">
+      <c r="H78" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="I78" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="H78" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="I78" s="9" t="s">
+      <c r="J78" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="J78" s="9" t="s">
-        <v>214</v>
-      </c>
       <c r="K78" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L78" s="9">
         <v>1979</v>
@@ -5792,31 +5778,31 @@
         <v>14</v>
       </c>
       <c r="C79" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D79" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D79" s="10" t="s">
+      <c r="E79" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F79" s="9" t="s">
         <v>216</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>217</v>
       </c>
       <c r="G79" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I79" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J79" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="J79" s="9" t="s">
+      <c r="K79" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="K79" s="9" t="s">
-        <v>220</v>
       </c>
       <c r="L79" s="9">
         <v>2001</v>
@@ -5840,26 +5826,26 @@
         <v>14</v>
       </c>
       <c r="C80" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D80" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="D80" s="10" t="s">
-        <v>222</v>
-      </c>
       <c r="E80" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I80" s="9" t="s">
         <v>42</v>
       </c>
       <c r="J80" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
@@ -5880,31 +5866,31 @@
         <v>14</v>
       </c>
       <c r="C81" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D81" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>225</v>
-      </c>
       <c r="E81" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="G81" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I81" s="9" t="s">
         <v>42</v>
       </c>
       <c r="J81" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K81" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L81" s="9">
         <v>1978</v>
@@ -5934,25 +5920,25 @@
         <v>28</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G82" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L82" s="9">
         <v>1978</v>
@@ -5982,25 +5968,25 @@
         <v>29</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="G83" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I83" s="9" t="s">
         <v>42</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L83" s="9">
         <v>1978</v>
@@ -6024,31 +6010,31 @@
         <v>14</v>
       </c>
       <c r="C84" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D84" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="D84" s="10" t="s">
+      <c r="E84" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F84" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>230</v>
       </c>
       <c r="G84" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>42</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L84" s="9">
         <v>1978</v>
@@ -6072,31 +6058,31 @@
         <v>14</v>
       </c>
       <c r="C85" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D85" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="D85" s="26" t="s">
-        <v>233</v>
-      </c>
       <c r="E85" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="G85" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I85" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L85" s="9">
         <v>1978</v>
@@ -6120,31 +6106,31 @@
         <v>14</v>
       </c>
       <c r="C86" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D86" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="D86" s="10" t="s">
-        <v>236</v>
-      </c>
       <c r="E86" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G86" s="9" t="s">
         <v>41</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I86" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L86" s="9">
         <v>2004</v>
@@ -6165,34 +6151,34 @@
     </row>
     <row r="87" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="D87" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="E87" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F87" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="G87" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="E87" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F87" s="9" t="s">
+      <c r="H87" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I87" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G87" s="9" t="s">
+      <c r="J87" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="H87" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I87" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J87" s="17" t="s">
-        <v>296</v>
-      </c>
       <c r="K87" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L87" s="37">
         <v>1970</v>
@@ -6213,34 +6199,34 @@
     </row>
     <row r="88" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C88" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F88" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="D88" s="10" t="s">
+      <c r="G88" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J88" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="E88" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="G88" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I88" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J88" s="17" t="s">
-        <v>300</v>
-      </c>
       <c r="K88" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L88" s="38">
         <v>1970</v>
@@ -6261,34 +6247,34 @@
     </row>
     <row r="89" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F89" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I89" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G89" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I89" s="9" t="s">
-        <v>295</v>
-      </c>
       <c r="J89" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K89" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L89" s="38">
         <v>1970</v>
@@ -6309,34 +6295,34 @@
     </row>
     <row r="90" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F90" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I90" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G90" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I90" s="9" t="s">
-        <v>295</v>
-      </c>
       <c r="J90" s="17" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L90" s="38">
         <v>1970</v>
@@ -6357,34 +6343,34 @@
     </row>
     <row r="91" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F91" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I91" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G91" s="9" t="s">
+      <c r="J91" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="H91" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I91" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J91" s="17" t="s">
-        <v>296</v>
-      </c>
       <c r="K91" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L91" s="38">
         <v>1970</v>
@@ -6405,34 +6391,34 @@
     </row>
     <row r="92" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C92" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F92" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="D92" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="E92" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>308</v>
-      </c>
       <c r="G92" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J92" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="H92" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I92" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J92" s="17" t="s">
-        <v>296</v>
-      </c>
       <c r="K92" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L92" s="38">
         <v>1970</v>
@@ -6453,34 +6439,34 @@
     </row>
     <row r="93" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F93" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I93" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G93" s="9" t="s">
+      <c r="J93" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="H93" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I93" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J93" s="17" t="s">
-        <v>296</v>
-      </c>
       <c r="K93" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L93" s="38">
         <v>1970</v>
@@ -6501,34 +6487,34 @@
     </row>
     <row r="94" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C94" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F94" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="D94" s="10" t="s">
+      <c r="G94" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I94" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="E94" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F94" s="9" t="s">
+      <c r="J94" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="G94" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I94" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="J94" s="17" t="s">
-        <v>315</v>
-      </c>
       <c r="K94" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L94" s="38">
         <v>1970</v>
@@ -6537,7 +6523,7 @@
         <v>2022</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O94" s="11" t="s">
         <v>32</v>
@@ -6549,34 +6535,34 @@
     </row>
     <row r="95" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C95" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F95" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="D95" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>319</v>
-      </c>
       <c r="G95" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J95" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L95" s="38">
         <v>1970</v>
@@ -6597,34 +6583,34 @@
     </row>
     <row r="96" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F96" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I96" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G96" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>295</v>
-      </c>
       <c r="J96" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K96" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L96" s="38">
         <v>1970</v>
@@ -6645,34 +6631,34 @@
     </row>
     <row r="97" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F97" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I97" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G97" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H97" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I97" s="9" t="s">
-        <v>295</v>
-      </c>
       <c r="J97" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K97" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L97" s="38">
         <v>1970</v>
@@ -6681,7 +6667,7 @@
         <v>2022</v>
       </c>
       <c r="N97" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O97" s="11" t="s">
         <v>32</v>
@@ -6693,34 +6679,34 @@
     </row>
     <row r="98" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C98" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="G98" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="D98" s="10" t="s">
+      <c r="H98" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I98" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J98" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="E98" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="G98" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I98" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J98" s="17" t="s">
-        <v>327</v>
-      </c>
       <c r="K98" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L98" s="38">
         <v>1970</v>
@@ -6741,34 +6727,34 @@
     </row>
     <row r="99" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C99" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G99" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="D99" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F99" s="9" t="s">
+      <c r="H99" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I99" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J99" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="G99" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="H99" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I99" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J99" s="17" t="s">
-        <v>331</v>
-      </c>
       <c r="K99" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L99" s="38">
         <v>1970</v>
@@ -6789,34 +6775,34 @@
     </row>
     <row r="100" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C100" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I100" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="D100" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F100" s="9" t="s">
+      <c r="J100" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G100" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I100" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="J100" s="9" t="s">
-        <v>335</v>
-      </c>
       <c r="K100" s="9" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="L100" s="38">
         <v>1996</v>
@@ -6825,7 +6811,7 @@
         <v>2022</v>
       </c>
       <c r="N100" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O100" s="11" t="s">
         <v>32</v>
@@ -6837,34 +6823,34 @@
     </row>
     <row r="101" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C101" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="G101" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="D101" s="10" t="s">
+      <c r="H101" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I101" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J101" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="E101" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="G101" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I101" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J101" s="9" t="s">
-        <v>339</v>
-      </c>
       <c r="K101" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="L101" s="38">
         <v>1970</v>
@@ -6885,34 +6871,34 @@
     </row>
     <row r="102" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C102" s="39" t="s">
+        <v>338</v>
+      </c>
+      <c r="D102" s="40" t="s">
+        <v>339</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I102" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J102" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="D102" s="40" t="s">
-        <v>341</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="G102" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I102" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J102" s="9" t="s">
-        <v>342</v>
-      </c>
       <c r="K102" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L102" s="38">
         <v>2012</v>
@@ -6933,34 +6919,34 @@
     </row>
     <row r="103" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C103" s="39" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D103" s="41" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I103" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K103" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L103" s="38">
         <v>2012</v>
@@ -6981,34 +6967,34 @@
     </row>
     <row r="104" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C104" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D104" s="41" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K104" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L104" s="38">
         <v>2012</v>
@@ -7029,34 +7015,34 @@
     </row>
     <row r="105" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C105" s="39" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I105" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J105" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L105" s="38">
         <v>2012</v>
@@ -7077,34 +7063,34 @@
     </row>
     <row r="106" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C106" s="39" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D106" s="41" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I106" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J106" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L106" s="38">
         <v>2012</v>
@@ -7125,34 +7111,34 @@
     </row>
     <row r="107" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C107" s="39" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D107" s="42" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I107" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J107" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L107" s="38">
         <v>2012</v>
@@ -7173,32 +7159,32 @@
     </row>
     <row r="108" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C108" s="39" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D108" s="41" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I108" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L108" s="38">
         <v>2012</v>
@@ -7219,34 +7205,34 @@
     </row>
     <row r="109" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C109" s="39" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D109" s="41" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I109" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K109" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L109" s="38">
         <v>2012</v>
@@ -7267,34 +7253,34 @@
     </row>
     <row r="110" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C110" s="39" t="s">
+        <v>355</v>
+      </c>
+      <c r="D110" s="41" t="s">
+        <v>356</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G110" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I110" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J110" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="D110" s="41" t="s">
-        <v>358</v>
-      </c>
-      <c r="E110" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="G110" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H110" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I110" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J110" s="9" t="s">
-        <v>359</v>
-      </c>
       <c r="K110" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L110" s="38">
         <v>2012</v>
@@ -7315,34 +7301,34 @@
     </row>
     <row r="111" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C111" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D111" s="41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I111" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K111" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L111" s="38">
         <v>2012</v>
@@ -7363,34 +7349,34 @@
     </row>
     <row r="112" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C112" s="39" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D112" s="41" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G112" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I112" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K112" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L112" s="38">
         <v>2012</v>
@@ -7411,34 +7397,34 @@
     </row>
     <row r="113" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D113" s="41" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G113" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I113" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K113" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L113" s="38">
         <v>2012</v>
@@ -7459,34 +7445,34 @@
     </row>
     <row r="114" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C114" s="39" t="s">
+        <v>361</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G114" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I114" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J114" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="D114" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="E114" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="G114" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I114" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J114" s="9" t="s">
-        <v>365</v>
-      </c>
       <c r="K114" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L114" s="38">
         <v>2012</v>
@@ -7507,34 +7493,34 @@
     </row>
     <row r="115" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C115" s="39" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D115" s="41" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I115" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K115" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L115" s="38">
         <v>2012</v>
@@ -7555,34 +7541,34 @@
     </row>
     <row r="116" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C116" s="39" t="s">
+        <v>366</v>
+      </c>
+      <c r="D116" s="41" t="s">
+        <v>367</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="G116" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I116" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J116" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="D116" s="41" t="s">
-        <v>369</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="G116" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H116" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I116" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J116" s="9" t="s">
-        <v>370</v>
-      </c>
       <c r="K116" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L116" s="38">
         <v>2012</v>
@@ -7603,34 +7589,34 @@
     </row>
     <row r="117" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C117" s="39" t="s">
+        <v>369</v>
+      </c>
+      <c r="D117" s="41" t="s">
+        <v>370</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="G117" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I117" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J117" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="D117" s="41" t="s">
-        <v>372</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F117" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="G117" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H117" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I117" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J117" s="9" t="s">
-        <v>373</v>
-      </c>
       <c r="K117" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="L117" s="38">
         <v>2012</v>
@@ -7651,31 +7637,31 @@
     </row>
     <row r="118" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C118" s="39" t="s">
+        <v>372</v>
+      </c>
+      <c r="D118" s="41" t="s">
+        <v>373</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F118" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="D118" s="41" t="s">
+      <c r="G118" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I118" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J118" s="9" t="s">
         <v>375</v>
-      </c>
-      <c r="E118" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F118" s="9" t="s">
-        <v>376</v>
-      </c>
-      <c r="G118" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H118" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I118" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J118" s="9" t="s">
-        <v>377</v>
       </c>
       <c r="K118" s="9">
         <v>2022</v>
@@ -7699,31 +7685,31 @@
     </row>
     <row r="119" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C119" s="39" t="s">
+        <v>376</v>
+      </c>
+      <c r="D119" s="41" t="s">
+        <v>377</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F119" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="D119" s="41" t="s">
+      <c r="G119" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I119" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J119" s="9" t="s">
         <v>379</v>
-      </c>
-      <c r="E119" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="F119" s="9" t="s">
-        <v>380</v>
-      </c>
-      <c r="G119" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I119" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="J119" s="9" t="s">
-        <v>381</v>
       </c>
       <c r="K119" s="9"/>
       <c r="L119" s="38"/>
@@ -7741,34 +7727,34 @@
     </row>
     <row r="120" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C120" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="D120" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F120" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="D120" s="10" t="s">
+      <c r="G120" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I120" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="E120" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F120" s="9" t="s">
+      <c r="J120" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="G120" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I120" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="J120" s="9" t="s">
-        <v>386</v>
-      </c>
       <c r="K120" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L120" s="38">
         <v>2019</v>

</xml_diff>

<commit_message>
add reviews received today and start addressing the issues raised by reviewers
</commit_message>
<xml_diff>
--- a/planning/Ageing-workshop-regional-homework-all-regions.xlsx
+++ b/planning/Ageing-workshop-regional-homework-all-regions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc-my.sharepoint.com/personal/daniel_ricard_dfo-mpo_gc_ca/Documents/Documents/GitHub/ageing-best-practices-2023/planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\GitHub\ageing-best-practices-2023\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{958294BC-080D-45F6-A58C-69867F9750FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876E77F2-BFB1-4C52-B7B1-1336F3468897}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DCC8D8-FCE6-4B9F-8E67-6BD58D2B2865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45120" yWindow="45" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="425">
   <si>
     <t>Region</t>
   </si>
@@ -1300,6 +1300,15 @@
   </si>
   <si>
     <t>2021 and 2022</t>
+  </si>
+  <si>
+    <t>OP/ARC</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>GLF</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1617,6 +1626,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1928,7 +1940,7 @@
     <tableColumn id="9" xr3:uid="{3D42B2E0-7DD8-452F-9B97-D1252951BE09}" name="Age validation study" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{519A576D-E865-420A-A674-ECFFC4F66206}" name="Reference collection" dataDxfId="1"/>
     <tableColumn id="14" xr3:uid="{4655E220-6EFE-49C3-89A6-C712327CE81A}" name="Region.short" dataDxfId="0">
-      <calculatedColumnFormula>UPPER(LEFT(Table2[[#This Row],[Region]],3))</calculatedColumnFormula>
+      <calculatedColumnFormula xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2322,9 +2334,8 @@
       <c r="O5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P5" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2370,9 +2381,8 @@
       <c r="O6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P6" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2418,9 +2428,8 @@
       <c r="O7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P7" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2466,9 +2475,8 @@
       <c r="O8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P8" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2514,9 +2522,8 @@
       <c r="O9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P9" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2562,9 +2569,8 @@
       <c r="O10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P10" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P10" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2610,9 +2616,8 @@
       <c r="O11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P11" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2658,9 +2663,8 @@
       <c r="O12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P12" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P12" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2706,9 +2710,8 @@
       <c r="O13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P13" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P13" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2754,9 +2757,8 @@
       <c r="O14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P14" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P14" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2802,9 +2804,8 @@
       <c r="O15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P15" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P15" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2850,9 +2851,8 @@
       <c r="O16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P16" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P16" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2898,9 +2898,8 @@
       <c r="O17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P17" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P17" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2946,9 +2945,8 @@
       <c r="O18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P18" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>GUL</v>
+      <c r="P18" s="3" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2993,7 +2991,7 @@
       </c>
       <c r="O19" s="11"/>
       <c r="P19" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3041,7 +3039,7 @@
         <v>20</v>
       </c>
       <c r="P20" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3089,7 +3087,7 @@
         <v>19</v>
       </c>
       <c r="P21" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3135,7 +3133,7 @@
       </c>
       <c r="O22" s="11"/>
       <c r="P22" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3183,7 +3181,7 @@
         <v>20</v>
       </c>
       <c r="P23" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3231,7 +3229,7 @@
         <v>19</v>
       </c>
       <c r="P24" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3275,7 +3273,7 @@
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3323,7 +3321,7 @@
         <v>263</v>
       </c>
       <c r="P26" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3363,7 +3361,7 @@
       </c>
       <c r="O27" s="11"/>
       <c r="P27" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3403,7 +3401,7 @@
       </c>
       <c r="O28" s="11"/>
       <c r="P28" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3447,7 +3445,7 @@
       </c>
       <c r="O29" s="11"/>
       <c r="P29" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3491,7 +3489,7 @@
       </c>
       <c r="O30" s="11"/>
       <c r="P30" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3535,7 +3533,7 @@
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3579,7 +3577,7 @@
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3623,7 +3621,7 @@
       </c>
       <c r="O33" s="11"/>
       <c r="P33" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>MAR</v>
       </c>
     </row>
@@ -3671,7 +3669,7 @@
         <v>19</v>
       </c>
       <c r="P34" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>QUE</v>
       </c>
     </row>
@@ -3719,7 +3717,7 @@
         <v>149</v>
       </c>
       <c r="P35" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>QUE</v>
       </c>
     </row>
@@ -3767,7 +3765,7 @@
         <v>149</v>
       </c>
       <c r="P36" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>QUE</v>
       </c>
     </row>
@@ -3811,7 +3809,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>QUE</v>
       </c>
     </row>
@@ -3859,7 +3857,7 @@
         <v>19</v>
       </c>
       <c r="P38" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>QUE</v>
       </c>
     </row>
@@ -3907,7 +3905,7 @@
         <v>103</v>
       </c>
       <c r="P39" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -3955,7 +3953,7 @@
         <v>103</v>
       </c>
       <c r="P40" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4003,7 +4001,7 @@
         <v>103</v>
       </c>
       <c r="P41" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4051,7 +4049,7 @@
         <v>103</v>
       </c>
       <c r="P42" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4099,7 +4097,7 @@
         <v>103</v>
       </c>
       <c r="P43" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4145,7 +4143,7 @@
       </c>
       <c r="O44" s="11"/>
       <c r="P44" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4193,7 +4191,7 @@
         <v>103</v>
       </c>
       <c r="P45" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4241,7 +4239,7 @@
         <v>103</v>
       </c>
       <c r="P46" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4289,7 +4287,7 @@
         <v>103</v>
       </c>
       <c r="P47" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4337,7 +4335,7 @@
         <v>103</v>
       </c>
       <c r="P48" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4385,7 +4383,7 @@
         <v>103</v>
       </c>
       <c r="P49" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4433,7 +4431,7 @@
         <v>103</v>
       </c>
       <c r="P50" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4481,7 +4479,7 @@
         <v>103</v>
       </c>
       <c r="P51" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4529,7 +4527,7 @@
         <v>103</v>
       </c>
       <c r="P52" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4577,7 +4575,7 @@
         <v>103</v>
       </c>
       <c r="P53" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4625,7 +4623,7 @@
         <v>103</v>
       </c>
       <c r="P54" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4671,7 +4669,7 @@
       </c>
       <c r="O55" s="11"/>
       <c r="P55" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4719,7 +4717,7 @@
         <v>103</v>
       </c>
       <c r="P56" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4767,7 +4765,7 @@
         <v>103</v>
       </c>
       <c r="P57" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4815,7 +4813,7 @@
         <v>103</v>
       </c>
       <c r="P58" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4863,7 +4861,7 @@
         <v>103</v>
       </c>
       <c r="P59" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4911,7 +4909,7 @@
         <v>103</v>
       </c>
       <c r="P60" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -4959,7 +4957,7 @@
         <v>103</v>
       </c>
       <c r="P61" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5007,7 +5005,7 @@
         <v>103</v>
       </c>
       <c r="P62" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5055,7 +5053,7 @@
         <v>103</v>
       </c>
       <c r="P63" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5103,7 +5101,7 @@
         <v>103</v>
       </c>
       <c r="P64" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5151,7 +5149,7 @@
         <v>103</v>
       </c>
       <c r="P65" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5199,7 +5197,7 @@
         <v>103</v>
       </c>
       <c r="P66" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5247,7 +5245,7 @@
         <v>103</v>
       </c>
       <c r="P67" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5295,7 +5293,7 @@
         <v>103</v>
       </c>
       <c r="P68" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5343,7 +5341,7 @@
         <v>103</v>
       </c>
       <c r="P69" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5391,7 +5389,7 @@
         <v>103</v>
       </c>
       <c r="P70" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
+        <f xml:space="preserve"> UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
         <v>PAC</v>
       </c>
     </row>
@@ -5438,9 +5436,8 @@
       <c r="O71" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P71" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P71" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="72" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5486,9 +5483,8 @@
       <c r="O72" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P72" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P72" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="73" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5532,9 +5528,8 @@
       <c r="O73" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="P73" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P73" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="74" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5578,9 +5573,8 @@
       <c r="O74" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="P74" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P74" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="75" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5626,9 +5620,8 @@
       <c r="O75" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P75" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P75" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="76" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5672,9 +5665,8 @@
       <c r="O76" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P76" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P76" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5720,9 +5712,8 @@
       <c r="O77" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="P77" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P77" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="78" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5768,9 +5759,8 @@
       <c r="O78" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P78" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P78" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="79" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5816,9 +5806,8 @@
       <c r="O79" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P79" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P79" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="80" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5856,9 +5845,8 @@
       <c r="O80" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P80" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P80" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="81" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5904,9 +5892,8 @@
       <c r="O81" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P81" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P81" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="82" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5952,9 +5939,8 @@
       <c r="O82" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P82" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P82" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="83" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6000,9 +5986,8 @@
       <c r="O83" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P83" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P83" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="84" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6048,9 +6033,8 @@
       <c r="O84" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P84" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P84" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="85" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6096,9 +6080,8 @@
       <c r="O85" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P85" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P85" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="86" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6144,9 +6127,8 @@
       <c r="O86" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P86" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>NEW</v>
+      <c r="P86" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="87" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6192,9 +6174,8 @@
       <c r="O87" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P87" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P87" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="88" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6240,9 +6221,8 @@
       <c r="O88" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P88" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P88" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="89" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6288,9 +6268,8 @@
       <c r="O89" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P89" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P89" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="90" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6336,9 +6315,8 @@
       <c r="O90" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P90" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P90" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="91" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6384,9 +6362,8 @@
       <c r="O91" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P91" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P91" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="92" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6432,9 +6409,8 @@
       <c r="O92" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P92" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P92" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="93" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6480,9 +6456,8 @@
       <c r="O93" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P93" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P93" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="94" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6528,9 +6503,8 @@
       <c r="O94" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P94" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P94" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="95" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6576,9 +6550,8 @@
       <c r="O95" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P95" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P95" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="96" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6624,9 +6597,8 @@
       <c r="O96" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P96" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P96" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="97" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6672,9 +6644,8 @@
       <c r="O97" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P97" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P97" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="98" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6720,9 +6691,8 @@
       <c r="O98" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P98" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P98" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="99" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6768,9 +6738,8 @@
       <c r="O99" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P99" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P99" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="100" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6816,9 +6785,8 @@
       <c r="O100" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P100" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P100" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="101" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6864,9 +6832,8 @@
       <c r="O101" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P101" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P101" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="102" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6912,9 +6879,8 @@
       <c r="O102" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P102" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P102" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="103" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6960,9 +6926,8 @@
       <c r="O103" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P103" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P103" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="104" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7008,9 +6973,8 @@
       <c r="O104" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P104" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P104" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7056,9 +7020,8 @@
       <c r="O105" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P105" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P105" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="106" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7104,9 +7067,8 @@
       <c r="O106" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P106" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P106" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="107" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7152,9 +7114,8 @@
       <c r="O107" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P107" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P107" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="108" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7198,9 +7159,8 @@
       <c r="O108" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P108" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P108" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="109" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7246,9 +7206,8 @@
       <c r="O109" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P109" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P109" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="110" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7294,9 +7253,8 @@
       <c r="O110" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P110" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P110" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="111" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7342,9 +7300,8 @@
       <c r="O111" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P111" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P111" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="112" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7390,9 +7347,8 @@
       <c r="O112" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P112" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P112" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="113" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7438,9 +7394,8 @@
       <c r="O113" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P113" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P113" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7486,9 +7441,8 @@
       <c r="O114" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P114" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P114" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7534,9 +7488,8 @@
       <c r="O115" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P115" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P115" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="116" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7582,9 +7535,8 @@
       <c r="O116" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P116" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P116" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="117" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7630,9 +7582,8 @@
       <c r="O117" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P117" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P117" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="118" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7678,9 +7629,8 @@
       <c r="O118" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P118" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P118" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="119" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7720,9 +7670,8 @@
       <c r="O119" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P119" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P119" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="120" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -7768,9 +7717,8 @@
       <c r="O120" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="P120" s="3" t="str">
-        <f>UPPER(LEFT(Table2[[#This Row],[Region]],3))</f>
-        <v>ONT</v>
+      <c r="P120" s="43" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update PDF of proceedings report and create date-stamped PDF to send for publication
</commit_message>
<xml_diff>
--- a/planning/Ageing-workshop-regional-homework-all-regions.xlsx
+++ b/planning/Ageing-workshop-regional-homework-all-regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\GitHub\ageing-best-practices-2023\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DCC8D8-FCE6-4B9F-8E67-6BD58D2B2865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2D9B5F-6244-481F-ADDA-509C20CCA537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45120" yWindow="45" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="424">
   <si>
     <t>Region</t>
   </si>
@@ -838,9 +838,6 @@
   </si>
   <si>
     <t>Sectioned Shell</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
   <si>
     <t>Sea Scallop</t>
@@ -2236,12 +2233,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2249,13 +2246,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>38</v>
@@ -2264,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>31</v>
@@ -2276,10 +2273,10 @@
         <v>3</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>37</v>
@@ -2288,7 +2285,7 @@
         <v>4</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2299,7 @@
         <v>24</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
@@ -2311,7 +2308,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>17</v>
@@ -2335,7 +2332,7 @@
         <v>19</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2349,7 +2346,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>11</v>
@@ -2358,7 +2355,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>17</v>
@@ -2382,7 +2379,7 @@
         <v>20</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2396,7 +2393,7 @@
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
@@ -2405,7 +2402,7 @@
         <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>17</v>
@@ -2429,7 +2426,7 @@
         <v>20</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2443,7 +2440,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
@@ -2452,7 +2449,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>17</v>
@@ -2476,7 +2473,7 @@
         <v>20</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2490,7 +2487,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>11</v>
@@ -2499,7 +2496,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>17</v>
@@ -2523,7 +2520,7 @@
         <v>20</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2537,7 +2534,7 @@
         <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>12</v>
@@ -2546,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>17</v>
@@ -2570,7 +2567,7 @@
         <v>32</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2584,7 +2581,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
@@ -2593,7 +2590,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>42</v>
@@ -2617,7 +2614,7 @@
         <v>32</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2631,7 +2628,7 @@
         <v>47</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>11</v>
@@ -2640,7 +2637,7 @@
         <v>41</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>42</v>
@@ -2664,7 +2661,7 @@
         <v>32</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2678,7 +2675,7 @@
         <v>48</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>11</v>
@@ -2687,7 +2684,7 @@
         <v>41</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>42</v>
@@ -2711,7 +2708,7 @@
         <v>32</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2725,7 +2722,7 @@
         <v>138</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>11</v>
@@ -2734,7 +2731,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>139</v>
@@ -2758,7 +2755,7 @@
         <v>32</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2772,16 +2769,16 @@
         <v>123</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>124</v>
@@ -2790,7 +2787,7 @@
         <v>125</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L15" s="3">
         <v>1983</v>
@@ -2805,7 +2802,7 @@
         <v>32</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2819,7 +2816,7 @@
         <v>127</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>128</v>
@@ -2828,7 +2825,7 @@
         <v>94</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>129</v>
@@ -2852,7 +2849,7 @@
         <v>32</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2866,7 +2863,7 @@
         <v>131</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>132</v>
@@ -2875,7 +2872,7 @@
         <v>13</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>124</v>
@@ -2884,7 +2881,7 @@
         <v>21</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="L17" s="3">
         <v>2021</v>
@@ -2899,7 +2896,7 @@
         <v>32</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2913,16 +2910,16 @@
         <v>134</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>135</v>
@@ -2946,7 +2943,7 @@
         <v>32</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2960,16 +2957,16 @@
         <v>24</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>17</v>
@@ -2978,7 +2975,7 @@
         <v>18</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L19" s="9">
         <v>1970</v>
@@ -3006,16 +3003,16 @@
         <v>24</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>17</v>
@@ -3024,7 +3021,7 @@
         <v>18</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L20" s="9">
         <v>1970</v>
@@ -3054,25 +3051,25 @@
         <v>138</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>142</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L21" s="12">
         <v>1954</v>
@@ -3081,7 +3078,7 @@
         <v>2022</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>19</v>
@@ -3102,16 +3099,16 @@
         <v>232</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>17</v>
@@ -3120,7 +3117,7 @@
         <v>18</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L22" s="9">
         <v>1970</v>
@@ -3148,16 +3145,16 @@
         <v>232</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>17</v>
@@ -3166,7 +3163,7 @@
         <v>18</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L23" s="9">
         <v>1970</v>
@@ -3190,22 +3187,22 @@
         <v>15</v>
       </c>
       <c r="C24" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>287</v>
-      </c>
       <c r="E24" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I24" s="14" t="s">
         <v>17</v>
@@ -3214,7 +3211,7 @@
         <v>18</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L24" s="16">
         <v>1970</v>
@@ -3244,23 +3241,23 @@
         <v>260</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>17</v>
       </c>
       <c r="J25" s="17"/>
       <c r="K25" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L25" s="9">
         <v>1975</v>
@@ -3288,7 +3285,7 @@
         <v>261</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>229</v>
@@ -3297,7 +3294,7 @@
         <v>13</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>262</v>
@@ -3336,14 +3333,14 @@
         <v>265</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="9" t="s">
         <v>95</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>266</v>
@@ -3351,9 +3348,7 @@
       <c r="J27" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="K27" s="9" t="s">
-        <v>268</v>
-      </c>
+      <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9" t="s">
@@ -3370,30 +3365,28 @@
         <v>15</v>
       </c>
       <c r="C28" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>270</v>
-      </c>
       <c r="E28" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="9" t="s">
         <v>95</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I28" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="J28" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="J28" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>268</v>
-      </c>
+      <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="9" t="s">
@@ -3416,20 +3409,20 @@
         <v>127</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I29" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="J29" s="17" t="s">
         <v>273</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>274</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>196</v>
@@ -3460,23 +3453,23 @@
         <v>123</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I30" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="J30" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="J30" s="17" t="s">
-        <v>274</v>
-      </c>
       <c r="K30" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L30" s="9">
         <v>1970</v>
@@ -3504,23 +3497,23 @@
         <v>131</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I31" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="J31" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="J31" s="17" t="s">
-        <v>274</v>
-      </c>
       <c r="K31" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L31" s="9">
         <v>1970</v>
@@ -3548,23 +3541,23 @@
         <v>134</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J32" s="9" t="s">
         <v>18</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L32" s="9">
         <v>1980</v>
@@ -3586,23 +3579,23 @@
         <v>15</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>277</v>
-      </c>
       <c r="E33" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J33" s="9" t="s">
         <v>18</v>
@@ -3636,7 +3629,7 @@
         <v>138</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>141</v>
@@ -3645,7 +3638,7 @@
         <v>13</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>142</v>
@@ -3684,7 +3677,7 @@
         <v>145</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>12</v>
@@ -3693,7 +3686,7 @@
         <v>13</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I35" s="9" t="s">
         <v>146</v>
@@ -3732,7 +3725,7 @@
         <v>150</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>151</v>
@@ -3741,7 +3734,7 @@
         <v>13</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>17</v>
@@ -3780,7 +3773,7 @@
         <v>228</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>12</v>
@@ -3789,7 +3782,7 @@
         <v>13</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>17</v>
@@ -3824,7 +3817,7 @@
         <v>24</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>237</v>
@@ -3833,7 +3826,7 @@
         <v>13</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>238</v>
@@ -3872,16 +3865,16 @@
         <v>65</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>153</v>
@@ -3920,16 +3913,16 @@
         <v>66</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I40" s="9" t="s">
         <v>153</v>
@@ -3968,16 +3961,16 @@
         <v>67</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>153</v>
@@ -4016,16 +4009,16 @@
         <v>68</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>153</v>
@@ -4064,16 +4057,16 @@
         <v>69</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>153</v>
@@ -4112,16 +4105,16 @@
         <v>158</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>153</v>
@@ -4158,16 +4151,16 @@
         <v>70</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>153</v>
@@ -4206,16 +4199,16 @@
         <v>71</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>153</v>
@@ -4254,16 +4247,16 @@
         <v>72</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I47" s="9" t="s">
         <v>153</v>
@@ -4302,16 +4295,16 @@
         <v>73</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I48" s="9" t="s">
         <v>153</v>
@@ -4350,16 +4343,16 @@
         <v>74</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I49" s="9" t="s">
         <v>153</v>
@@ -4398,16 +4391,16 @@
         <v>76</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I50" s="9" t="s">
         <v>153</v>
@@ -4446,16 +4439,16 @@
         <v>77</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I51" s="9" t="s">
         <v>153</v>
@@ -4494,16 +4487,16 @@
         <v>78</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I52" s="9" t="s">
         <v>153</v>
@@ -4542,16 +4535,16 @@
         <v>79</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I53" s="9" t="s">
         <v>153</v>
@@ -4590,16 +4583,16 @@
         <v>80</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I54" s="9" t="s">
         <v>153</v>
@@ -4638,16 +4631,16 @@
         <v>161</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I55" s="9" t="s">
         <v>153</v>
@@ -4684,16 +4677,16 @@
         <v>111</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I56" s="9" t="s">
         <v>153</v>
@@ -4732,16 +4725,16 @@
         <v>81</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G57" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I57" s="9" t="s">
         <v>153</v>
@@ -4780,16 +4773,16 @@
         <v>82</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>93</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I58" s="9" t="s">
         <v>164</v>
@@ -4828,16 +4821,16 @@
         <v>83</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I59" s="9" t="s">
         <v>153</v>
@@ -4876,7 +4869,7 @@
         <v>118</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>166</v>
@@ -4885,7 +4878,7 @@
         <v>13</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I60" s="9" t="s">
         <v>42</v>
@@ -4924,7 +4917,7 @@
         <v>84</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>168</v>
@@ -4933,7 +4926,7 @@
         <v>94</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I61" s="9" t="s">
         <v>17</v>
@@ -4972,7 +4965,7 @@
         <v>85</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>170</v>
@@ -4981,7 +4974,7 @@
         <v>94</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I62" s="9" t="s">
         <v>164</v>
@@ -5020,7 +5013,7 @@
         <v>86</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>172</v>
@@ -5029,7 +5022,7 @@
         <v>94</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I63" s="9" t="s">
         <v>164</v>
@@ -5068,7 +5061,7 @@
         <v>87</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>174</v>
@@ -5077,7 +5070,7 @@
         <v>94</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I64" s="9" t="s">
         <v>164</v>
@@ -5116,7 +5109,7 @@
         <v>88</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>176</v>
@@ -5125,7 +5118,7 @@
         <v>94</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I65" s="9" t="s">
         <v>164</v>
@@ -5164,7 +5157,7 @@
         <v>89</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>178</v>
@@ -5173,7 +5166,7 @@
         <v>94</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I66" s="9" t="s">
         <v>17</v>
@@ -5212,7 +5205,7 @@
         <v>90</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>180</v>
@@ -5221,7 +5214,7 @@
         <v>95</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I67" s="9" t="s">
         <v>121</v>
@@ -5260,7 +5253,7 @@
         <v>91</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>182</v>
@@ -5269,7 +5262,7 @@
         <v>95</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I68" s="9" t="s">
         <v>183</v>
@@ -5308,7 +5301,7 @@
         <v>92</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>180</v>
@@ -5317,7 +5310,7 @@
         <v>95</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I69" s="9" t="s">
         <v>183</v>
@@ -5356,7 +5349,7 @@
         <v>116</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F70" s="29" t="s">
         <v>187</v>
@@ -5365,7 +5358,7 @@
         <v>95</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I70" s="29" t="s">
         <v>117</v>
@@ -5404,7 +5397,7 @@
         <v>189</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>190</v>
@@ -5413,7 +5406,7 @@
         <v>13</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I71" s="9" t="s">
         <v>191</v>
@@ -5437,7 +5430,7 @@
         <v>32</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="72" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5451,7 +5444,7 @@
         <v>138</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>193</v>
@@ -5460,7 +5453,7 @@
         <v>13</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I72" s="9" t="s">
         <v>194</v>
@@ -5484,7 +5477,7 @@
         <v>32</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="73" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5498,16 +5491,16 @@
         <v>24</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G73" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I73" s="9" t="s">
         <v>17</v>
@@ -5526,10 +5519,10 @@
       </c>
       <c r="N73" s="9"/>
       <c r="O73" s="11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="P73" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="74" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5543,16 +5536,16 @@
         <v>26</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I74" s="9" t="s">
         <v>17</v>
@@ -5571,10 +5564,10 @@
       </c>
       <c r="N74" s="9"/>
       <c r="O74" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="75" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5588,7 +5581,7 @@
         <v>198</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>199</v>
@@ -5597,7 +5590,7 @@
         <v>13</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I75" s="9" t="s">
         <v>17</v>
@@ -5621,7 +5614,7 @@
         <v>19</v>
       </c>
       <c r="P75" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5635,7 +5628,7 @@
         <v>25</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>201</v>
@@ -5644,7 +5637,7 @@
         <v>13</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I76" s="9" t="s">
         <v>202</v>
@@ -5666,7 +5659,7 @@
         <v>19</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="77" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5680,16 +5673,16 @@
         <v>127</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F77" s="35" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G77" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I77" s="35" t="s">
         <v>205</v>
@@ -5713,7 +5706,7 @@
         <v>19</v>
       </c>
       <c r="P77" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="78" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5727,7 +5720,7 @@
         <v>209</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>210</v>
@@ -5736,7 +5729,7 @@
         <v>211</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I78" s="9" t="s">
         <v>212</v>
@@ -5760,7 +5753,7 @@
         <v>19</v>
       </c>
       <c r="P78" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="79" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5774,7 +5767,7 @@
         <v>215</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>216</v>
@@ -5783,7 +5776,7 @@
         <v>13</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I79" s="9" t="s">
         <v>217</v>
@@ -5807,7 +5800,7 @@
         <v>32</v>
       </c>
       <c r="P79" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="80" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5821,14 +5814,14 @@
         <v>221</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I80" s="9" t="s">
         <v>42</v>
@@ -5846,7 +5839,7 @@
         <v>32</v>
       </c>
       <c r="P80" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="81" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5860,16 +5853,16 @@
         <v>224</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G81" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I81" s="9" t="s">
         <v>42</v>
@@ -5893,7 +5886,7 @@
         <v>32</v>
       </c>
       <c r="P81" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="82" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5907,7 +5900,7 @@
         <v>28</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>225</v>
@@ -5916,7 +5909,7 @@
         <v>13</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I82" s="9" t="s">
         <v>226</v>
@@ -5940,7 +5933,7 @@
         <v>32</v>
       </c>
       <c r="P82" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="83" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5954,16 +5947,16 @@
         <v>29</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G83" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I83" s="9" t="s">
         <v>42</v>
@@ -5987,7 +5980,7 @@
         <v>32</v>
       </c>
       <c r="P83" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="84" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6001,7 +5994,7 @@
         <v>228</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F84" s="9" t="s">
         <v>229</v>
@@ -6010,7 +6003,7 @@
         <v>13</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I84" s="9" t="s">
         <v>42</v>
@@ -6034,7 +6027,7 @@
         <v>32</v>
       </c>
       <c r="P84" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="85" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6048,16 +6041,16 @@
         <v>232</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G85" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I85" s="9" t="s">
         <v>233</v>
@@ -6081,7 +6074,7 @@
         <v>32</v>
       </c>
       <c r="P85" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="86" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -6095,7 +6088,7 @@
         <v>235</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F86" s="9" t="s">
         <v>216</v>
@@ -6104,7 +6097,7 @@
         <v>41</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I86" s="9" t="s">
         <v>217</v>
@@ -6128,39 +6121,39 @@
         <v>32</v>
       </c>
       <c r="P86" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="87" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="C87" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="D87" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="E87" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F87" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="E87" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F87" s="9" t="s">
+      <c r="G87" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G87" s="9" t="s">
+      <c r="H87" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I87" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H87" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I87" s="9" t="s">
+      <c r="J87" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="J87" s="17" t="s">
-        <v>294</v>
-      </c>
       <c r="K87" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L87" s="37">
         <v>1970</v>
@@ -6175,39 +6168,39 @@
         <v>32</v>
       </c>
       <c r="P87" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="88" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C88" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D88" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="D88" s="10" t="s">
+      <c r="E88" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F88" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="E88" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F88" s="9" t="s">
+      <c r="G88" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J88" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="G88" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I88" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J88" s="17" t="s">
-        <v>298</v>
-      </c>
       <c r="K88" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L88" s="38">
         <v>1970</v>
@@ -6222,39 +6215,39 @@
         <v>32</v>
       </c>
       <c r="P88" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="89" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C89" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D89" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="D89" s="10" t="s">
-        <v>300</v>
-      </c>
       <c r="E89" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F89" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G89" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G89" s="9" t="s">
+      <c r="H89" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I89" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H89" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I89" s="9" t="s">
-        <v>293</v>
-      </c>
       <c r="J89" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K89" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L89" s="38">
         <v>1970</v>
@@ -6269,39 +6262,39 @@
         <v>32</v>
       </c>
       <c r="P89" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="90" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F90" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G90" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G90" s="9" t="s">
+      <c r="H90" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I90" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H90" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I90" s="9" t="s">
-        <v>293</v>
-      </c>
       <c r="J90" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L90" s="38">
         <v>1970</v>
@@ -6316,39 +6309,39 @@
         <v>32</v>
       </c>
       <c r="P90" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="91" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C91" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D91" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="D91" s="10" t="s">
-        <v>303</v>
-      </c>
       <c r="E91" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F91" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G91" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G91" s="9" t="s">
+      <c r="H91" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I91" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H91" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I91" s="9" t="s">
+      <c r="J91" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="J91" s="17" t="s">
-        <v>294</v>
-      </c>
       <c r="K91" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L91" s="38">
         <v>1970</v>
@@ -6363,39 +6356,39 @@
         <v>32</v>
       </c>
       <c r="P91" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="92" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C92" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D92" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="E92" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F92" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="E92" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>306</v>
-      </c>
       <c r="G92" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I92" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H92" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I92" s="9" t="s">
+      <c r="J92" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="J92" s="17" t="s">
-        <v>294</v>
-      </c>
       <c r="K92" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L92" s="38">
         <v>1970</v>
@@ -6410,39 +6403,39 @@
         <v>32</v>
       </c>
       <c r="P92" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="93" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C93" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D93" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="D93" s="10" t="s">
-        <v>308</v>
-      </c>
       <c r="E93" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F93" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G93" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G93" s="9" t="s">
+      <c r="H93" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I93" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H93" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I93" s="9" t="s">
+      <c r="J93" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="J93" s="17" t="s">
-        <v>294</v>
-      </c>
       <c r="K93" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L93" s="38">
         <v>1970</v>
@@ -6457,39 +6450,39 @@
         <v>32</v>
       </c>
       <c r="P93" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="94" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C94" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="D94" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="D94" s="10" t="s">
+      <c r="E94" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F94" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="E94" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F94" s="9" t="s">
+      <c r="G94" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I94" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="G94" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I94" s="9" t="s">
+      <c r="J94" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="J94" s="17" t="s">
-        <v>313</v>
-      </c>
       <c r="K94" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L94" s="38">
         <v>1970</v>
@@ -6498,45 +6491,45 @@
         <v>2022</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O94" s="11" t="s">
         <v>32</v>
       </c>
       <c r="P94" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="95" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C95" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="D95" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="D95" s="10" t="s">
+      <c r="E95" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F95" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="E95" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>317</v>
-      </c>
       <c r="G95" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I95" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H95" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>293</v>
-      </c>
       <c r="J95" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K95" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L95" s="38">
         <v>1970</v>
@@ -6551,39 +6544,39 @@
         <v>32</v>
       </c>
       <c r="P95" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="96" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C96" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="D96" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="D96" s="10" t="s">
-        <v>319</v>
-      </c>
       <c r="E96" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F96" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G96" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G96" s="9" t="s">
+      <c r="H96" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I96" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H96" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>293</v>
-      </c>
       <c r="J96" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K96" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L96" s="38">
         <v>1970</v>
@@ -6598,39 +6591,39 @@
         <v>32</v>
       </c>
       <c r="P96" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="97" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C97" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="D97" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="D97" s="10" t="s">
-        <v>321</v>
-      </c>
       <c r="E97" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F97" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G97" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G97" s="9" t="s">
+      <c r="H97" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I97" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="H97" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I97" s="9" t="s">
-        <v>293</v>
-      </c>
       <c r="J97" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K97" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L97" s="38">
         <v>1970</v>
@@ -6639,45 +6632,45 @@
         <v>2022</v>
       </c>
       <c r="N97" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O97" s="11" t="s">
         <v>32</v>
       </c>
       <c r="P97" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="98" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C98" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D98" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D98" s="10" t="s">
+      <c r="E98" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="G98" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="E98" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="G98" s="9" t="s">
+      <c r="H98" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I98" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J98" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="H98" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I98" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J98" s="17" t="s">
-        <v>325</v>
-      </c>
       <c r="K98" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L98" s="38">
         <v>1970</v>
@@ -6692,39 +6685,39 @@
         <v>32</v>
       </c>
       <c r="P98" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="99" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C99" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F99" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="D99" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F99" s="9" t="s">
+      <c r="G99" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="G99" s="9" t="s">
+      <c r="H99" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I99" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J99" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="H99" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I99" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J99" s="17" t="s">
-        <v>329</v>
-      </c>
       <c r="K99" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L99" s="38">
         <v>1970</v>
@@ -6739,39 +6732,39 @@
         <v>32</v>
       </c>
       <c r="P99" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="100" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>198</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F100" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I100" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="G100" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I100" s="9" t="s">
+      <c r="J100" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="J100" s="9" t="s">
-        <v>333</v>
-      </c>
       <c r="K100" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L100" s="38">
         <v>1996</v>
@@ -6780,45 +6773,45 @@
         <v>2022</v>
       </c>
       <c r="N100" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O100" s="11" t="s">
         <v>32</v>
       </c>
       <c r="P100" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="101" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C101" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="D101" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D101" s="10" t="s">
+      <c r="E101" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="G101" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="E101" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="G101" s="9" t="s">
+      <c r="H101" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I101" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J101" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="H101" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I101" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J101" s="9" t="s">
-        <v>337</v>
-      </c>
       <c r="K101" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L101" s="38">
         <v>1970</v>
@@ -6833,39 +6826,39 @@
         <v>32</v>
       </c>
       <c r="P101" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="102" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C102" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="D102" s="40" t="s">
         <v>338</v>
       </c>
-      <c r="D102" s="40" t="s">
+      <c r="E102" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I102" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J102" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E102" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="G102" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I102" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J102" s="9" t="s">
-        <v>340</v>
-      </c>
       <c r="K102" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L102" s="38">
         <v>2012</v>
@@ -6880,39 +6873,39 @@
         <v>32</v>
       </c>
       <c r="P102" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="103" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C103" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="D103" s="41" t="s">
         <v>341</v>
       </c>
-      <c r="D103" s="41" t="s">
-        <v>342</v>
-      </c>
       <c r="E103" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I103" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K103" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L103" s="38">
         <v>2012</v>
@@ -6927,39 +6920,39 @@
         <v>32</v>
       </c>
       <c r="P103" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C104" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="D104" s="41" t="s">
         <v>343</v>
       </c>
-      <c r="D104" s="41" t="s">
-        <v>344</v>
-      </c>
       <c r="E104" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K104" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L104" s="38">
         <v>2012</v>
@@ -6974,39 +6967,39 @@
         <v>32</v>
       </c>
       <c r="P104" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="105" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C105" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="D105" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="D105" s="10" t="s">
-        <v>346</v>
-      </c>
       <c r="E105" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I105" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J105" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L105" s="38">
         <v>2012</v>
@@ -7021,39 +7014,39 @@
         <v>32</v>
       </c>
       <c r="P105" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="106" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C106" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="D106" s="41" t="s">
         <v>347</v>
       </c>
-      <c r="D106" s="41" t="s">
-        <v>348</v>
-      </c>
       <c r="E106" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I106" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J106" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L106" s="38">
         <v>2012</v>
@@ -7068,39 +7061,39 @@
         <v>32</v>
       </c>
       <c r="P106" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="107" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C107" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="D107" s="42" t="s">
         <v>349</v>
       </c>
-      <c r="D107" s="42" t="s">
-        <v>350</v>
-      </c>
       <c r="E107" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I107" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J107" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L107" s="38">
         <v>2012</v>
@@ -7115,37 +7108,37 @@
         <v>32</v>
       </c>
       <c r="P107" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="108" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C108" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="D108" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="D108" s="41" t="s">
-        <v>352</v>
-      </c>
       <c r="E108" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I108" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J108" s="9"/>
       <c r="K108" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L108" s="38">
         <v>2012</v>
@@ -7160,39 +7153,39 @@
         <v>32</v>
       </c>
       <c r="P108" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C109" s="39" t="s">
+        <v>352</v>
+      </c>
+      <c r="D109" s="41" t="s">
         <v>353</v>
       </c>
-      <c r="D109" s="41" t="s">
-        <v>354</v>
-      </c>
       <c r="E109" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I109" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K109" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L109" s="38">
         <v>2012</v>
@@ -7207,39 +7200,39 @@
         <v>32</v>
       </c>
       <c r="P109" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="110" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C110" s="39" t="s">
+        <v>354</v>
+      </c>
+      <c r="D110" s="41" t="s">
         <v>355</v>
       </c>
-      <c r="D110" s="41" t="s">
+      <c r="E110" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G110" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I110" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J110" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="E110" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="G110" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H110" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I110" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J110" s="9" t="s">
-        <v>357</v>
-      </c>
       <c r="K110" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L110" s="38">
         <v>2012</v>
@@ -7254,12 +7247,12 @@
         <v>32</v>
       </c>
       <c r="P110" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="111" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C111" s="39" t="s">
         <v>144</v>
@@ -7268,25 +7261,25 @@
         <v>189</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I111" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K111" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L111" s="38">
         <v>2012</v>
@@ -7301,39 +7294,39 @@
         <v>32</v>
       </c>
       <c r="P111" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="112" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C112" s="39" t="s">
+        <v>357</v>
+      </c>
+      <c r="D112" s="41" t="s">
         <v>358</v>
       </c>
-      <c r="D112" s="41" t="s">
-        <v>359</v>
-      </c>
       <c r="E112" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G112" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I112" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K112" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L112" s="38">
         <v>2012</v>
@@ -7348,39 +7341,39 @@
         <v>32</v>
       </c>
       <c r="P112" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="113" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D113" s="41" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G113" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I113" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K113" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L113" s="38">
         <v>2012</v>
@@ -7395,39 +7388,39 @@
         <v>32</v>
       </c>
       <c r="P113" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="114" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C114" s="39" t="s">
+        <v>360</v>
+      </c>
+      <c r="D114" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="D114" s="10" t="s">
+      <c r="E114" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G114" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I114" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J114" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="E114" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="G114" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I114" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J114" s="9" t="s">
-        <v>363</v>
-      </c>
       <c r="K114" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L114" s="38">
         <v>2012</v>
@@ -7442,39 +7435,39 @@
         <v>32</v>
       </c>
       <c r="P114" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="115" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C115" s="39" t="s">
+        <v>363</v>
+      </c>
+      <c r="D115" s="41" t="s">
         <v>364</v>
       </c>
-      <c r="D115" s="41" t="s">
-        <v>365</v>
-      </c>
       <c r="E115" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I115" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K115" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L115" s="38">
         <v>2012</v>
@@ -7489,39 +7482,39 @@
         <v>32</v>
       </c>
       <c r="P115" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="116" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C116" s="39" t="s">
+        <v>365</v>
+      </c>
+      <c r="D116" s="41" t="s">
         <v>366</v>
       </c>
-      <c r="D116" s="41" t="s">
+      <c r="E116" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="G116" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I116" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J116" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="E116" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="G116" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H116" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I116" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J116" s="9" t="s">
-        <v>368</v>
-      </c>
       <c r="K116" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L116" s="38">
         <v>2012</v>
@@ -7536,39 +7529,39 @@
         <v>32</v>
       </c>
       <c r="P116" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="117" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C117" s="39" t="s">
+        <v>368</v>
+      </c>
+      <c r="D117" s="41" t="s">
         <v>369</v>
       </c>
-      <c r="D117" s="41" t="s">
+      <c r="E117" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="G117" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I117" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J117" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="E117" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="F117" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="G117" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H117" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I117" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J117" s="9" t="s">
-        <v>371</v>
-      </c>
       <c r="K117" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L117" s="38">
         <v>2012</v>
@@ -7583,36 +7576,36 @@
         <v>32</v>
       </c>
       <c r="P117" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="118" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C118" s="39" t="s">
+        <v>371</v>
+      </c>
+      <c r="D118" s="41" t="s">
         <v>372</v>
       </c>
-      <c r="D118" s="41" t="s">
+      <c r="E118" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F118" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="E118" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F118" s="9" t="s">
+      <c r="G118" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I118" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J118" s="9" t="s">
         <v>374</v>
-      </c>
-      <c r="G118" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H118" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I118" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J118" s="9" t="s">
-        <v>375</v>
       </c>
       <c r="K118" s="9">
         <v>2022</v>
@@ -7630,36 +7623,36 @@
         <v>32</v>
       </c>
       <c r="P118" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="119" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C119" s="39" t="s">
+        <v>375</v>
+      </c>
+      <c r="D119" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="D119" s="41" t="s">
+      <c r="E119" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="F119" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="E119" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F119" s="9" t="s">
+      <c r="G119" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I119" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="J119" s="9" t="s">
         <v>378</v>
-      </c>
-      <c r="G119" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I119" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="J119" s="9" t="s">
-        <v>379</v>
       </c>
       <c r="K119" s="9"/>
       <c r="L119" s="38"/>
@@ -7671,36 +7664,36 @@
         <v>32</v>
       </c>
       <c r="P119" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="120" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C120" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="D120" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="D120" s="10" t="s">
+      <c r="E120" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F120" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="E120" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="F120" s="9" t="s">
+      <c r="G120" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I120" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="G120" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="I120" s="9" t="s">
+      <c r="J120" s="9" t="s">
         <v>383</v>
-      </c>
-      <c r="J120" s="9" t="s">
-        <v>384</v>
       </c>
       <c r="K120" s="9" t="s">
         <v>188</v>
@@ -7718,7 +7711,7 @@
         <v>32</v>
       </c>
       <c r="P120" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>